<commit_message>
Fixed numerous bugs, added facets
</commit_message>
<xml_diff>
--- a/data/AI Conference Agenda.xlsx
+++ b/data/AI Conference Agenda.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,12 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="4658" windowHeight="4380"/>
   </bookViews>
   <sheets>
-    <sheet name="AI Conference Agenda" sheetId="1" r:id="rId1"/>
-    <sheet name="Speakers" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Monday AI Conference Agenda" sheetId="1" r:id="rId1"/>
+    <sheet name="Tuesday AI Conference Agenda" sheetId="4" r:id="rId2"/>
+    <sheet name="Speakers" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="213">
   <si>
     <t>Title</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Workshop: Machine Learning in the Enterprise – Open to All Attendees</t>
   </si>
   <si>
-    <t>Intelligent Assistants &amp; Bots – What You Need to Know</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -50,11 +47,6 @@
     <t>Creds</t>
   </si>
   <si>
-    <t>The Machine Learning Market
-Today: The Who, What and Why of
-Enterprise ML</t>
-  </si>
-  <si>
     <t xml:space="preserve">1:00PM </t>
   </si>
   <si>
@@ -70,21 +62,9 @@
     <t>Data Scientist</t>
   </si>
   <si>
-    <t>Expo Opens</t>
-  </si>
-  <si>
-    <t>AI World Executive Summit</t>
-  </si>
-  <si>
     <t>Track</t>
   </si>
   <si>
-    <t>Workshop - Building an Application-Specific Bot</t>
-  </si>
-  <si>
-    <t>Workshop - Machine Learning in the Enterprise</t>
-  </si>
-  <si>
     <t>Links</t>
   </si>
   <si>
@@ -238,9 +218,6 @@
     <t>digitate</t>
   </si>
   <si>
-    <t>Bot Workshop Second Half</t>
-  </si>
-  <si>
     <t xml:space="preserve">JP (Jean-Pierre) Abello, Beena Ammanath, Mark Bünger, Linda Bernardi,  Micheal Chui, Dr. Neil Eklund, David Ledbetter, Danny Lange, Dr. Harrick Vin, </t>
   </si>
   <si>
@@ -250,9 +227,6 @@
     <t>Building the Ecosystem: Investment, Alliances and Partnering</t>
   </si>
   <si>
-    <t>General Session Panel</t>
-  </si>
-  <si>
     <t>Umair Akeel, Chris Farmer, Tim Chang, Patrick Eggen</t>
   </si>
   <si>
@@ -334,44 +308,374 @@
     <t>Monday</t>
   </si>
   <si>
-    <t>State-of-the-Practice in ML
-for the Enterprise</t>
-  </si>
-  <si>
-    <t>3:15PM</t>
-  </si>
-  <si>
-    <t>Jan Lasek, Robert Bogucki, Manohar Paluri,  Ravi Srivatsav</t>
-  </si>
-  <si>
-    <t>Example event</t>
-  </si>
-  <si>
-    <t>4:00PM</t>
-  </si>
-  <si>
-    <t>John Smith, Ryan Volum</t>
-  </si>
-  <si>
-    <t>Pretend Workshop</t>
-  </si>
-  <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>Panel of four world class heads of machine
-learning will present what they are doing
-at their companies, how ML is disrupting
-their industries, and critical lessons learned
-in deploying enterprise class machine
-learning applications.</t>
+    <t>Pre-Conference Workshop</t>
+  </si>
+  <si>
+    <t>ML in the Enterprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intelligent Assistants &amp; Bots </t>
+  </si>
+  <si>
+    <t>AI Executive Summit</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/workshop-machine-learning/</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/workshop-building-bot/</t>
+  </si>
+  <si>
+    <t>AI Executive Summit Child</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>AI Executive Summit intro</t>
+  </si>
+  <si>
+    <t>As artificial intelligence technologies such as machine learning and robotics start to become more prevalent, their potential effect on the workplace has become a major focus of academic, business, and public concern. We will discuss findings from our detailed research that show that the story is more nuanced than simply asking whether mass unemployment is just around the corner.</t>
+  </si>
+  <si>
+    <t>Michael Chui</t>
+  </si>
+  <si>
+    <t>This year will long be remembered as the breakout year for AI, with new technologies and applications growing up faster than it seemed possible to track. Like a teenager who’s just earned the right to car keys, AI’s responsibilities and the consequences of its actions permanently passed a milestone in 2016. Our panel will discuss the significant events that show how AI is leaving adolescence – and what it’s likely to be up next. Join our executive panelists to hear how we got here, what’s most important now, and what 2017 will hold in store.</t>
+  </si>
+  <si>
+    <t>Moderator</t>
+  </si>
+  <si>
+    <t>Beena Ammanath, Dr. Neil Eklund, Kumar Srivastava</t>
+  </si>
+  <si>
+    <t>Through all the hype about artificial intelligence, how is it relevant for your enterprise IT? Why should you care? In this session, we will examine the long running challenges IT has in managing complex business critical applications and the infrastructure. Learn how AI can finally solve these complex issues and transform your organization to be substantially more agile!</t>
+  </si>
+  <si>
+    <t>Akhilesh Tripathi</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence, Automation, Activities and Occupations – What the Future Could Hold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Executive Panel: 2016 – The Year AI Grew Up </t>
+  </si>
+  <si>
+    <t>Why is Artificial Intelligence Relevant for IT?</t>
+  </si>
+  <si>
+    <t>A Deep Learning Approach to Understanding Critical Illness in Children</t>
+  </si>
+  <si>
+    <t>Mr. Ledbetter will discuss how his team applies recurrent neural networks to learn important correlations within the electronic health records of over 20,000 patients from the Pediatric Intensive Care Unit at Children’s Hospital Los Angeles over a period of more than 10 years. The learned models predict the trajectory of patient vitals and probability of survival. The models enable a clinician to insert a therapy and assess whether the vital and mortality predictions are perturbed in a useful fashion.</t>
+  </si>
+  <si>
+    <t>Break</t>
+  </si>
+  <si>
+    <t>In a devastatingly incisive article in 2003, Harvard Business Review stated bluntly, “IT Doesn’t Matter.” After a decade of treating information technology as a competitive differentiator, the fact that IT had become ubiquitous and affordable to all meant that it was no longer a strategic matter, capable of changing the fate of one company over its peers. But today, artificial intelligence has the potential to once again give companies something that their competitors can’t copy, and can’t beat. But will it, who will do it, how will it happen, and when? Our executive panel lay out the promising points, and a path to get there.</t>
+  </si>
+  <si>
+    <t>JP (Jean-Pierre) Abello, Danny Lange, David Linthicum</t>
+  </si>
+  <si>
+    <t>Will AI Make IT a Strategic Differentiator Again?</t>
+  </si>
+  <si>
+    <t> AI: What Lies Ahead?</t>
+  </si>
+  <si>
+    <t>These days AI finds itself in sentences with words like “breakthrough” and “finally real”. There have indeed been great advances in key areas like object and speech recognition, language translation, and predictive analytics. But AI is much more than that. Demographic trends like the aging population and technical trends like the Internet of Things require new ways of thinking about human-machine interaction and trustable autonomy. AI’s biggest impact lies ahead.</t>
+  </si>
+  <si>
+    <t>Dr. William Mark</t>
+  </si>
+  <si>
+    <t>Fireside Chat</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Cyril Magnin 3</t>
+  </si>
+  <si>
+    <t>Cyril Magnin 2</t>
+  </si>
+  <si>
+    <t>General Session</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/building-ecosystem/</t>
+  </si>
+  <si>
+    <t>The AI and machine learning industries are in their infancy. As the market grows and expands, companies will need to continue to invest, build multi-industry channels and find unique and mutually beneficial partnerships in order to build enterprise-class business models.  In this session, veteran industry investment professionals discuss likely scenarios of how and where this will unfold, and where new investment opportunities will arise.</t>
+  </si>
+  <si>
+    <t>Cyril Magnin Ballroom</t>
+  </si>
+  <si>
+    <t>AI World Exhibition</t>
+  </si>
+  <si>
+    <t>Attack of the Bots – Demo Night and Ecosystem Panel</t>
+  </si>
+  <si>
+    <t>In this installment of MobileMonday we will see some live demos of Chatbots and Ecosystem Services supporting them.    We’ll follow demos with an ecosystem panel discussion.</t>
+  </si>
+  <si>
+    <t>Mario Tapia</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/mobile-monday/</t>
+  </si>
+  <si>
+    <t>Paul Walsh, Arte Merritt, Lauren Kunze, Alex Quintana</t>
+  </si>
+  <si>
+    <t>AI Startup Lightning Panel</t>
+  </si>
+  <si>
+    <t>Join AI start-up advisor Steve Ardire who will moderate this panel with 8 AI startups.  Each panelist will present their innovative AI-powered application, followed by an interactive panel of experts who will provide unbiased feedback along with audience Q&amp;A</t>
+  </si>
+  <si>
+    <t>Steve Ardire</t>
+  </si>
+  <si>
+    <t>Dr. Sindhu Joseph, Tamer Rashad, Nick Brestoff, Mounir Shita, Kristina Messdaghi, Maria Grineva, Dalia Asterbadi</t>
+  </si>
+  <si>
+    <t>Investors</t>
+  </si>
+  <si>
+    <t>Samad Farid, Shelley Zhuang, Christie Pitts</t>
+  </si>
+  <si>
+    <t>Enteprise AI Adoption: A Study of Vertical Industry Adoption – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>AI World and Rethink Research recently published “Enterprise AI Adoption: An Executive Guide on the Commercial Impact of AI and Machine Learning in Vertical Industries“, a research study based on a global survey of enterprises and an expert analysis of the state of the enterprise AI market –
+The potential impact and benefits of using artificial intelligence technologies such as machine learning, computer vision, natural language processing, predictive APIs and others are huge. McKinsey estimates the global economic impact of just one of the disruptive trends enabled by AI – automation of knowledge work – will be as great as $6.7 trillion by 2025. However, only some organizations are currently getting value from these technologies.
+This session will step thru some of the results of the study, including a comparision of vertical market adoption in a multitude of industries, the implementation phases that organizations are experiencing and what impact it is having on their business.</t>
+  </si>
+  <si>
+    <t>Caroline Gabriel</t>
+  </si>
+  <si>
+    <t>Special Event</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/enteprise-ai-adoption-open-attendees/</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/ai-startup-lightning-panel/</t>
+  </si>
+  <si>
+    <t>Cyril Magnin 1</t>
+  </si>
+  <si>
+    <t>Continental Breakfast</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/continental-breakfast-hosted-workfusion/</t>
+  </si>
+  <si>
+    <t>Hosted by WorkFusion</t>
+  </si>
+  <si>
+    <t>Adam Devine</t>
+  </si>
+  <si>
+    <t>Conference Welcome</t>
+  </si>
+  <si>
+    <t>AI World Conference and Expo brings together the industry’s thought leaders for an in-depth dive into the many facets of the business and technology of enterprise AI.
+On the first day of the main conference proram we focus on enterprise implementation and deployment strategies &amp; technologies.  The morning keynotes and general sessions explore key areas that large organizations need to address such as enterprise challenges for AI adoption, the role of cloud solutions vs. outsourced vs. home grown machine learning, how to assemble technology building blocks, and tracks covering the business and technology of AI and machine learning.</t>
+  </si>
+  <si>
+    <t>Mark Bunger, Eliot Weinman</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/program/</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: The State of AI</t>
+  </si>
+  <si>
+    <t>AI industry executives discuss the state of the practice of enterprise AI today, from “where we’re at” to “where we’re going”. The panel will examine the dynamics of the leading edge of the technology ecosystem and the associated cross-industry business impacts they are driving.</t>
+  </si>
+  <si>
+    <t>Dr. Neil Eklund, Stephen Pratt, Ashish Lahoti, Dr. William Mark, Jim McHugh</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/stat-of-artificial-intelligence/</t>
+  </si>
+  <si>
+    <t>Keynote</t>
+  </si>
+  <si>
+    <t>Dr. Michael Chui</t>
+  </si>
+  <si>
+    <t>Artificial intelligence, automation, activities and occupations – what the future could hold</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/keynote-2/</t>
+  </si>
+  <si>
+    <t>Coffee Break with Exhibitors</t>
+  </si>
+  <si>
+    <t>Practical AI Fueled by Big Data</t>
+  </si>
+  <si>
+    <t>Much like cloud computing and big data in the past decade, the current AI wave of innovation has its foundation in decades old concepts.  The enablers that created major industry inflection points around cloud and big data – open source, open standards, and powerful commodity hardware – will also drive hyper-growth of AI based applications and services.   Hear application case studies from Boyd Davis, CEO of Kogentix and Mike Olson, Chief Strategy Officer of Cloudera, how the rapidly evolving Cloudera Enterprise data hub, built on Hadoop and related open source components, is enabling companies to deliver machine learning on an enterprise scale.</t>
+  </si>
+  <si>
+    <t>Boyd Davis, Mike Olson</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/keynote-3/</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: Evolution or Disruption</t>
+  </si>
+  <si>
+    <t>Robert Bogucki, Anju Gupta, Danny Lange, Rahul Kelkar,General Session</t>
+  </si>
+  <si>
+    <t>Mark Bunger</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/executive-roundtable-enterprise-challenges-ai-adoption/</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/keynote-rob-high-ibm-fellow-vice-president-chief-technology-officer-ibm-watson/</t>
+  </si>
+  <si>
+    <t>Rob High</t>
+  </si>
+  <si>
+    <t>Keynote: Rob High, IBM Fellow, Vice President and Chief Technology Officer, IBM Watson</t>
+  </si>
+  <si>
+    <t>Keynote: Accelerating Industrial IoT with Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>An innovative technology leader with over 23 years proven track record of building core big data/data science competencies and leading high performance teams from the ground-up scaling 0 to 150+ geographically distributed global teams with a sharp focus on strategy and successful execution of industrial scale data science products and services. Experienced at recognized international organizations British Telecom, E*trade, Thomson Reuters, Bank of America and also, Silicon Valley startups, in engineering and management positions. She holds a Masters in Computer Science and MBA in Finance. Beena is dedicated to supporting diversity in technology both within GE and beyond. Outside of GE, she is on the Board of Directors for the non-profit organization, ChickTech.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/keynote-4/</t>
+  </si>
+  <si>
+    <t>Conference Luncheon and Network with Exhibitors</t>
+  </si>
+  <si>
+    <t>Lunch sponsored by pwc</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Deploying AI Business Systems</t>
+  </si>
+  <si>
+    <t>Finding the Best Applications for AI and Machine Learning1:30 PM</t>
+  </si>
+  <si>
+    <t>There are hundreds of AI and machine learning vendors promoting thousands of potential business applications for machine learning and associated technologies.  In addition, as enterprises move their workforce to the cloud, the major cloud vendors have been integrating machine learning software into their cloud offerings.</t>
+  </si>
+  <si>
+    <t>David Linthicum, Matt Zeiler, Jai Malhotra, Adam Devine</t>
+  </si>
+  <si>
+    <t>Cirrus Shakeri</t>
+  </si>
+  <si>
+    <t>How AI is Shaping the Future of the Auto &amp; Transportation Industries</t>
+  </si>
+  <si>
+    <t>Once a domain solely of human control, AI has found a place “behind the wheel” of personal and public transportation.  Learn how AI is powering this change, the obstacles it faces and what’s on the horizon of intelligent transportation.</t>
+  </si>
+  <si>
+    <t>Maryanna Saenko, Danny Shapiro</t>
+  </si>
+  <si>
+    <t>Industry Applications</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/ai-future-automotive-transportation/</t>
+  </si>
+  <si>
+    <t>State of Machine Learning 3.0</t>
+  </si>
+  <si>
+    <t>For the past two years, Shivon Ziis and Bloomberg Data has published their fall update on the state of machine intelligence. To date, this landscape has become the the industry’s leading comprehensive analysis on the entire landscape of the machine intelligence industry. Join authors Shivon Zilis and James Cham for as they discuss the current state-of-the-market of their latest report, Machine Intelligence 3.0.</t>
+  </si>
+  <si>
+    <t>James Chan, Shivon Zilis</t>
+  </si>
+  <si>
+    <t>The Technologies of Enterprise AI</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/state-of-machine-learning-3-0-ai/</t>
+  </si>
+  <si>
+    <t>AI in Industry</t>
+  </si>
+  <si>
+    <t>David Schubmehl moderates this panel of end-users and solution providers and will uncover a variety of innovative AI and machine learning applications being used in various industries, the technologies and platforms used, and also what approach these companies are using to deploy an enterprise implementation process.</t>
+  </si>
+  <si>
+    <t>Andrea L. Cardozo, JP (Jean-Pierre) Abello, David Parsin, Joseph Voyles, Reynold Xin</t>
+  </si>
+  <si>
+    <t>David Schubmehl</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/ai-in-industry/</t>
+  </si>
+  <si>
+    <t>Advances in Machine Learning</t>
+  </si>
+  <si>
+    <t>Advances in machine learning, deep learning and neural networks are transforming data management and decision making in almost every industry sector from retail to security and healthcare. These experts will discuss real world implementation challenges.</t>
+  </si>
+  <si>
+    <t>Derek Collison, Neil Eklund, Jennifer Marsman, Samir Vasavada</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/sessions/panel-advances-machine-learning/</t>
+  </si>
+  <si>
+    <t>Clint Wheelock</t>
+  </si>
+  <si>
+    <t>Driving Deep Learning Adoption Within the Enterprise</t>
+  </si>
+  <si>
+    <t>Fiaz Mohamed, Anju Gupta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep learning is in the early stages of unlocking tremendous economic value. While the algorithms have revolutionized consumer experiences in domains as varied as speech interfaces, image search and language translation, enterprises are still relatively early in their adoption of deep learning algorithms to solve broader business problems. The panelists will discuss the challenges of adopting deep learning based solutions within the enterprise and the need for a platform-based approach to AI deployment. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +697,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -411,24 +723,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -753,84 +1072,110 @@
     <col min="4" max="4" width="19.265625" customWidth="1"/>
     <col min="5" max="5" width="18.53125" customWidth="1"/>
     <col min="6" max="6" width="38.796875" customWidth="1"/>
-    <col min="7" max="7" width="31.86328125" customWidth="1"/>
+    <col min="7" max="7" width="68.9296875" customWidth="1"/>
+    <col min="11" max="11" width="31.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>96</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2" s="3">
         <v>0.54166666666666663</v>
       </c>
       <c r="C2" s="3">
-        <v>0.61458333333333337</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
-        <v>0.61458333333333337</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>94</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+      <c r="I3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="B4" s="3">
         <v>0.54166666666666663</v>
@@ -839,137 +1184,979 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4">
+        <v>102</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="D5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" t="s">
+        <v>126</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" t="s">
+        <v>126</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" t="s">
+        <v>126</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="F10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="3">
         <v>0.61458333333333337</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C14" s="3">
         <v>0.63541666666666663</v>
       </c>
-      <c r="H5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.63541666666666663</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="F14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="3">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="C15" s="3">
         <v>0.73958333333333337</v>
       </c>
-      <c r="E9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="2"/>
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="J16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="D17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" t="s">
+        <v>140</v>
+      </c>
+      <c r="K17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="D18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" t="s">
+        <v>147</v>
+      </c>
+      <c r="G18" t="s">
+        <v>148</v>
+      </c>
+      <c r="H18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A18" r:id="rId1" display="http://aiworldexpo.com/sessions/enteprise-ai-adoption-open-attendees/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="45.3984375" customWidth="1"/>
+    <col min="5" max="5" width="26.06640625" customWidth="1"/>
+    <col min="6" max="6" width="15.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.34375</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="F6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E8" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" t="s">
+        <v>175</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>131</v>
+      </c>
+      <c r="J8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" t="s">
+        <v>176</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D10" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" t="s">
+        <v>184</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" t="s">
+        <v>188</v>
+      </c>
+      <c r="F12" t="s">
+        <v>185</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" t="s">
+        <v>150</v>
+      </c>
+      <c r="J12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="D13" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" t="s">
+        <v>194</v>
+      </c>
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="D14" t="s">
+        <v>196</v>
+      </c>
+      <c r="E14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F14" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D15" t="s">
+        <v>201</v>
+      </c>
+      <c r="E15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E16" t="s">
+        <v>207</v>
+      </c>
+      <c r="F16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" t="s">
+        <v>208</v>
+      </c>
+      <c r="H16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D17" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" t="s">
+        <v>185</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" display="http://aiworldexpo.com/sessions/keynote-2/"/>
+    <hyperlink ref="A12" r:id="rId2" display="http://aiworldexpo.com/sessions/finding-best-applications-ai-machine-learning/"/>
+    <hyperlink ref="A13" r:id="rId3" display="http://aiworldexpo.com/sessions/ai-future-automotive-transportation/"/>
+    <hyperlink ref="A16" r:id="rId4" display="http://aiworldexpo.com/sessions/panel-advances-machine-learning/"/>
+    <hyperlink ref="A17" r:id="rId5" display="http://aiworldexpo.com/sessions/titans-emerge-cloud-computing/"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -984,294 +2171,294 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>86</v>
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>93</v>
+        <v>83</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1280,7 +2467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A23"/>
   <sheetViews>
@@ -1292,117 +2479,117 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Speakers to Conference List
</commit_message>
<xml_diff>
--- a/data/AI Conference Agenda.xlsx
+++ b/data/AI Conference Agenda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4658" windowHeight="4380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4658" windowHeight="4380" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Monday AI Conference Agenda" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="531">
   <si>
     <t>Title</t>
   </si>
@@ -89,12 +89,6 @@
     <t>TMA Associates</t>
   </si>
   <si>
-    <t>Christina Apatow</t>
-  </si>
-  <si>
-    <t>VP of Client Solutions</t>
-  </si>
-  <si>
     <t>API.ai</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>Jennifer Marsman</t>
   </si>
   <si>
-    <t>Dev. Evangelist</t>
-  </si>
-  <si>
     <t>Microsoft</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t>Author, Entrepreneur, Innovator</t>
   </si>
   <si>
-    <t>Micheal Chui</t>
-  </si>
-  <si>
     <t>Partner</t>
   </si>
   <si>
@@ -209,12 +197,6 @@
     <t>Uber</t>
   </si>
   <si>
-    <t>Dr. Harrick Vin</t>
-  </si>
-  <si>
-    <t>Vice President and Chief Scientist</t>
-  </si>
-  <si>
     <t>digitate</t>
   </si>
   <si>
@@ -257,9 +239,6 @@
     <t>Patrick Eggen</t>
   </si>
   <si>
-    <t>Head of Ventures Norht America</t>
-  </si>
-  <si>
     <t>Qualcomm Ventures</t>
   </si>
   <si>
@@ -269,12 +248,6 @@
     <t>http://aiworldexpo.com/wp-content/uploads/2016/06/aiworld_speakers_janlasek.jpg</t>
   </si>
   <si>
-    <t>Chief Science Officer</t>
-  </si>
-  <si>
-    <t>Deepsense.io</t>
-  </si>
-  <si>
     <t>Robert is the Chief Science Officer of Deepsense.io where he manages the R&amp;D team and focuses on deep learning and mathematical research. He started his professional career as a software engineer at UBS. Prior to joining deepsense.io, he worked on Big Data and Machine Learning problems as a project manager at CodiLime.  Robert is a dual major holding Master degrees in Mathematics and Computer Science from University of Warsaw. His interests include probability theory, functional analysis and theoretical computer science, which became a subject of his publications. He is also a successful Kaggle competitor.</t>
   </si>
   <si>
@@ -282,9 +255,6 @@
   </si>
   <si>
     <t>Sessions</t>
-  </si>
-  <si>
-    <t>Executive Roundtable: Evolution or Disruption?, Workshop: Machine Learning in the Enterprise – Open to All Attendees</t>
   </si>
   <si>
     <t>startTime</t>
@@ -669,13 +639,1098 @@
   </si>
   <si>
     <t xml:space="preserve">Deep learning is in the early stages of unlocking tremendous economic value. While the algorithms have revolutionized consumer experiences in domains as varied as speech interfaces, image search and language translation, enterprises are still relatively early in their adoption of deep learning algorithms to solve broader business problems. The panelists will discuss the challenges of adopting deep learning based solutions within the enterprise and the need for a platform-based approach to AI deployment. </t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_williammeisel.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t>William Meisel, Ph.D., president, TMA Associates (www.tmaa.com), is publisher and editor of LUI News (commerce developments in the language user interface).  LUI News was originally Speech Strategy News (a paid-subscription monthly newsletter launched in 1993). Dr. Meisel is author of the 2013 book, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="6"/>
+        <color rgb="FF595959"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The Software Society</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6"/>
+        <color rgb="FF595959"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, and its associated blog, and a consultant on market and product opportunities created by the maturing of speech technology. His experience in speech technology includes founding and running a speech recognition company. Meisel is organizer of the Mobile Voice Conference as Executive Director of the non-profit Applied Voice Input Output Society (AVIOS). Meisel has a B.S. in Engineering from Caltech and a Ph.D. in Electrical Engineering from USC. He began his career as a professor of Electrical Engineering and Computer Science and published the first technical book on computer pattern recognition.</t>
+    </r>
+  </si>
+  <si>
+    <t>Panel: Bots &amp; Beyond: The Future of intelligent Assistants</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/JP-Abello-website.jpg</t>
+  </si>
+  <si>
+    <t>JP Abello is part of Nielsen’s thought leadership team, where he currently leads Global Engineering R&amp;D for the Internet of Things, Connected TV and Digital Media.
+Before Nielsen, JP spent over two decades building innovative products used by millions of consumers worldwide, including Yahoo Connected TV which won an Engineering Emmy Award in 2011, and the OCAP application platform deployed in many US of set-top boxes.
+JP recently published a featured article on IoT in the Nielsen Journal of Measurement, and has given talks on consumer measurement at IoT World, AI Summit, IoT Security Summit, Smart Home Summit, TAB OOH Ratings, Media Ratings Council and Apps World.
+JP is also the co-chair of the Privacy &amp; Security sub-committee for the IoT Consortium, and an active member of the W3C, IAB, ATSC, CTA, TV Academy and serves as a judge for the CES Innovation Awards and the Emmy Awards.</t>
+  </si>
+  <si>
+    <t>Panel: AI in Industry</t>
+  </si>
+  <si>
+    <t>Andy Peart is CMO of Artificial Solutions, an international business specializing in Natural Language Interaction (NLI) – a form of AI-technology that allows people to talk to applications and electronic devices in free-format, multi-modal natural language. The company’s Teneo NLI development and analytics platform enables sophisticated natural language applications to be created in record time without the need for specialist linguistic skills. Since the company was formed in 2001, it has implemented hundreds of projects globally in 35 languages that are used by millions of people every year.
+A regular speaker at industry events including Mobile Voice Conference, LT-Accelerate and IA Conference, Andy delivers insight about current NLI implementations, the challenges businesses face and the future of natural language.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/Andy-Peart-photo.jpg</t>
+  </si>
+  <si>
+    <t>Seminar: Intelligent Assistants &amp; Bots</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Jeff-Adams.jpg</t>
+  </si>
+  <si>
+    <t>Jeff left Amazon in September, 2014 to establish Cobalt Speech &amp; Language, a new, independent, commercial speech &amp; language lab. Jeff Adams has been managing top-level speech &amp; language technology research for 20 years. Until 6 years ago, he worked at Nuance / Dragon, where he was responsible for developing &amp; improving the speech recognition that went into Nuance’s “Dragon” dictation software. He presided over many of the key improvements in the 1990s and 2000s that brought this technology into the mainstream and enabled widespread adoption.
+Jeff left Nuance in 2009 for Yap. Yap’s business was cloud-based speech recognition, primarily for the voicemail-to-text market. Under Jeff’s oversight, Yap built a world-class research group to go head-to-head against the much bigger companies that dominated the market, including at least one that used thousands of off-shore human transcribers.
+Over a period of 2 1/2 years, Jeff assembled a remarkable team of 12 exceptionally talented &amp; respected speech scientists, unprecedented for a small startup, and within a year or two, bested all of Yap’s competitors on an unbiased test set, and matched the performance of (off-shore) human transcription. That is the first and (so far) only known example of fully automatic speech recognition matching human performance. Yap’s success attracted the attention of Amazon, and Jeff and his team of 12 scientists moved to Amazon in 2011, forming the core of Amazon’s new speech &amp; language research lab.
+At Amazon, Jeff led efforts to build one of the industry’s leading speech &amp; language groups. That team is building speech and language solutions such as Echo, Fire TV and Dash.
+Jeff is the author of 25 patents and several published research papers.</t>
+  </si>
+  <si>
+    <t>Developer Evangelist</t>
+  </si>
+  <si>
+    <t>Jennifer Marsman is a Principal Software Development Engineer in Microsoft’s Developer and Platform Evangelism group, where she educates developers on Microsoft’s new technologies. In this role, Jennifer is a frequent speaker at software development conferences around the world. In 2016, Jennifer was recognized as one of the “top 100 most influential individuals in artificial intelligence and machine learning” by Onalytica. She has been featured in Bloomberg for her work using EEG and machine learning to perform lie detection. In 2009, Jennifer was chosen as “Techie whose innovation will have the biggest impact” by X-OLOGY for her work with GiveCamps, a weekend-long event where developers code for charity. She has also received many honors from Microsoft, including the “Best in Role” award for Technical Evangelism, Central Region Top Contributor Award, Heartland District Top Contributor Award, DPE Community Evangelist Award, CPE Champion Award, MSUS Diversity &amp; Inclusion Award, Gold Club, and Platinum Club. Prior to becoming a Developer Evangelist, Jennifer was a software developer in Microsoft’s Natural Interactive Services division. In this role, she earned two patents for her work in search and data mining algorithms. Jennifer has also held positions with Ford Motor Company, National Instruments, and Soar Technology. Jennifer holds a Bachelor’s Degree in Computer Engineering and Master’s Degree in Computer Science and Engineering from the University of Michigan in Ann Arbor. Her graduate work specialized in artificial intelligence and computational theory. Jennifer blogs at http://blogs.msdn.com/jennifer and tweets at http://twitter.com/jennifermarsman.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/Jennifer-Marsman-website.jpg</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: Evolution or Disruption?</t>
+  </si>
+  <si>
+    <t>Manohar Paluri is currently a Research Lead at Facebook AI research and manages the Computer Vision team in the Applied Machine Learning organization. He is passionate about Computer Vision and in the longer term goal of building systems that can perceive the way humans do. In the process of working on various perception efforts throughout his career he spent considerable time looking at Computer Vision problems in Industry and Academia. He worked at renowned places like Google Research, IBM Watson Research Labs, Stanford Research Institute before helping co found Facebook AI Research directed by Dr. Yann Lecun at Facebook.  Manohar spent his formative years at IIIT Hyderabad where he finished his undergraduate studies with Honors in Computer Vision and joined Georgia Tech. to pursue his Ph.D. For over a decade he has been working on various problems related to Perception and has made various contributions through his publications at CVPR, ICCV, ECCV, ICLR, KDD, IROS, ACCV etc. He is passionate about building real world systems that are used by billions of people that bring positive value at scale. Some of these systems are running at Facebook and already have tremendous impact in how people communicate using Facebook.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/Manohar-Paluri.jpg</t>
+  </si>
+  <si>
+    <t>Seminar: Machine Learning in the Enterprise – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Ravi-Srivatsav.png</t>
+  </si>
+  <si>
+    <t>Ravi is Chief Business Development Officer at NTT Innovation Institute Inc. (NTT i3), the prestigious Silicon Valley-based innovation center for NTT Group, one of the world’s largest ICT companies. He is responsible for all aspects of product marketing, sales and business development of software defined networks, Fog computing and machine learning products established at NTT i3.
+Accelerating the movement of innovation from initial idea to marketplace implementation, NTT i3 combines access to the significant global infrastructure resources, investment fund, research knowledge, and trusted long-standing customer relationships of NTT Global with its own software startup expertise and deep enterprise relationships.
+Prior to NTT i3, Ravi was the founder and CEO of ElasticBox, an enterprise startup designed to manage application workloads in a hybrid cloud infrastructure. The company was acquired by Century Link, a global communications, hosting, cloud and IT services company enabling customers to transform their businesses and their lives through innovative technology solutions.
+Ravi began his career in the technology sector as a product developer and product manager in enterprise software working with Rational Software, IBM and Microsoft. Additionally, he was the head of platforms and games in leading gaming companies including My Space (Fox Interactive Media) and Social Gaming Network (SGN).</t>
+  </si>
+  <si>
+    <t>Beena Ammanath is VP, Data and Analytics at General Electric. She works across the GE businesses and external customers to accelerate data science adoption leveraging big data technologies on Predix, GE’s Industrial IoT platform via revenue generating data and analytics products.
+A seasoned technology leader with over 23 years proven track record of building core big data/data science competencies and leading high performance teams from the ground-up scaling 0 to 150+ geographically distributed global teams with a sharp focus on strategy and successful execution of industrial scale data science products and services. Experienced at recognized international organizations British Telecom,
+E*trade, Thomson Reuters, Bank of America and also, Silicon Valley startups, in engineering and management positions. She holds a Masters in Computer Science and MBA in Finance. Beena is dedicated to supporting diversity in technology both within GE and beyond. Outside of GE, she is on the Board of Directors for the non-profit organization, ChickTech.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/Beena-Amanath.jpg</t>
+  </si>
+  <si>
+    <t>Mark Bünger, conference co-chair, joined Lux Research in 2005.  As a VP of Research he focuses on strategic planning and advanced technologies in bio-, aero-, and energy domains. Over 20 years and across 40 countries, he has worked as a management consultant, technology analyst, and entrepreneur at Accenture, Forrester Research, and several startups. He has served as chairman of the Swedish-American Chamber of Commerce, and guest lectures at the University of California Berkeley.
+Mark studied business at Mälardalen Polytechnic (Sweden) and the University of Texas at Austin, and studied and worked in neurology and bioengineering labs at the University of California San Francisco (UCSF). He is an avid linguist, athlete, and Maker.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_markbunger.jpg</t>
+  </si>
+  <si>
+    <t>Until very recently Linda was Chief Innovation Officer at IBM. Her passion is to disrupt in order to innovate globally across large enterprises and startups. Linda is an avid entrepreneur and startup investor across the globe. In 2001 she founded her startup which enabled the mass adoption of RFID technology and IoT (sold to Oracle Corporation). Linda is passionate about big data, cognitive, AI , machine learning and our highly disrupted future Connected World. Her book ProVoke discusses the Culture of Innovation and Disruption. She is a columnist with the Washington Post. As for Not for Profit passions, she is founding member of the Anita Borg Institute for Women and Technology and the SETI Institute in Astronomical Sciences.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_lindabernardi.jpg</t>
+  </si>
+  <si>
+    <t>Dr. Michael Chui is a partner at the McKinsey Global Institute (MGI), McKinsey’s business and economics research arm. He leads research on the impact of information technologies and innovation on business, the economy, and society. Michael has led McKinsey research in such areas as automation, data and analytics, social and collaboration technologies, and the Internet of Things.
+Michael is a frequent speaker at major global conferences, and his research has been cited in leading publications around the world. His PhD dissertation, entitled “I Still Haven’t Found What I’m Looking For: Web Searching as Query Refinement,” examined Web user search behaviors and the usability of Web search engines.
+As a McKinsey consultant, Michael served clients in the high-tech, media, and telecom industries on strategy, innovation and product development, IT, sales and marketing, M&amp;A, and organization.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/Michael_Chui_263x273fin.jpg</t>
+  </si>
+  <si>
+    <t>Panel: Bots &amp; Beyond: The Future of intelligent Assistants| Seminar: Intelligent Assistants &amp; Bots</t>
+  </si>
+  <si>
+    <t>Panel: AI in Industry| AI Executive Summit</t>
+  </si>
+  <si>
+    <t>Panel: Advances in Machine Learning| Seminar: Intelligent Assistants &amp; Bots</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: Evolution or Disruption?| Seminar: Machine Learning in the Enterprise – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>Keynote: Accelerating Industrial IoT with Artificial Intelligence| AI Executive Summit</t>
+  </si>
+  <si>
+    <t>AI Executive Summit, Executive Roundtable: Evolution or Disruption?| Industry Expert Wrap-Up| Panel: How AI is Shaping the Future of the Auto &amp; Transportation Industries| Conference Welcome| Day Three Conference Introduction</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: The State of AI| AI Executive Summit</t>
+  </si>
+  <si>
+    <t>Keynote: Artificial intelligence, automation, activities and occupations – what the future could hold| AI Executive Summit</t>
+  </si>
+  <si>
+    <t>Dr. Neil Eklund is one of the foremost scientists in the field of Asset Health Management, and an experienced technologist in the space of data science, industrial analytics, and machine learning, with over 20 years experience in developing fielded solutions to practical industrial problems. Neil is one of the founders of the Prognostics and Health Management Society, the preeminent professional association in the AHM field, and continues to serve on its board of directors. He was the first Editor in Chief of the International Journal of Prognostics and Health Management, responsible for both launching the journal and establishing it as the premier publication for AHM academics and practitioners to disseminate their research findings. Neil is also an active standards author within the International Standards Organization (ISO) in the field of diagnostics and prognostics for complex machinery.
+For the last two years, Neil has served as the Chief Data Scientist for Schlumberger, the world’s leading provider of technology for reservoir characterization, drilling, production, and processing to the oil and gas industry. Neil transformed the AHM program at Schlumberger, establishing the first successful deployed Internet of Things application in the oil industry which generated $20MM+ in the first three months of operation. For the 12 years prior to that, Neil was a research scientist in the Machine Learning laboratory of General Electric Global Research, where he gained deep technical experience across multiple industry segments, including Aerospace, Energy, Healthcare, Oil &amp; Gas, Financial, and Rail. Additionally, Neil has worked closely with a wide range of external customers include Defense Advanced Research Projects Agency (DARPA), National Aeronautics and Space Administration (NASA), Lockheed Martin, ExxonMobil, Ford Motor Company, and Boeing.
+Neil holds both a Ph.D. and a Masters degree from Rensselaer Polytechnic Institute. He holds eight patents, with another nine pending, and over 70 technical publications. Neil was a graduate-level university Machine Learning instructor for six years, and continues to teach classes for Schlumberger and the PHM Society.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/04/eklund263x273v1.jpg</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: The State of AI| AI Executive Summit|Panel: Advances in Machine Learning</t>
+  </si>
+  <si>
+    <t>Mr. David Ledbetter has an extensive and deep understanding of decision theory. He has experience implementing various decision engines, including convolutional neural networks, recurrent neural networks, random forests, extra trees, and linear discrimination analysis. His particular area of focus is in performance estimation, where he has demonstrated a tremendous ability to accurately predict performance on new data in nonstationary, real-world scenarios. David has worked on a number of real-world detection projects, including detecting circulating tumor cells in blood, automatic target recognition utilizing CNNs from satellite imagery, make/model car classification for the Los Angeles Police Department using CNNs, and acoustic right whale call detection from underwater sonobuoys. Recently, David has been developing RNNs to generate personalized treatment recommendations to optimize patient outcomes using unstructured electronic medical records from 10 years of data collected from the Children’s Hospital Los Angeles Pediatric Intensive Care Unit.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/David-Ledbetter-website.jpg</t>
+  </si>
+  <si>
+    <t>Panel: AI and Cognitive Computing in Healthcare| AI Executive Summit</t>
+  </si>
+  <si>
+    <t>A serial innovator of large-scale distributed software systems with significant breakthroughs in cloud-based Machine Learning, MapReduce, Mobile-to-Cloud architectures, Mobile Search, Distributed Speech Recognition, Mobile Agents, and Hypertext.
+At Uber, we are building a world-class Machine Learning team. At Amazon Danny ran the internal Machine Learning platform (EML) and launched Amazon Machine Learning for AWS. Machine Learning is one of the amazing technologies that sets Amazon apart from its competitors.
+Highly motivated, self-starting individual who has contributed in both startups and large companies. Known as a skillful engineering leader who favors agile development with a strong drive for daily progress.
+Founder of Vocomo Software in 2001. Vocomo technology platform acquried by Google in 2005. Vocomo customer base acquired by Voxeo same year.
+Accomplished author and speaker; author of numerous patents.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_dannylange.jpg</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: Evolution or Disruption?| AI Executive Summit</t>
+  </si>
+  <si>
+    <t>Umair Akeel is the Chief Technology Officer In-Residence and Operating Partner at Bessemer Venture Partners. Umair brings 15 years of experience in technology development and leadership to Bessemer, focusing on SaaS. He is also passionate about the applications of machine learning to our everyday lives like self driving cars. Prior to joining Bessemer, Umair was Eloqua’s chief architect through its IPO and subsequent acquisition by Oracle (where he served as VP of product development).</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/umair-273x263.jpg</t>
+  </si>
+  <si>
+    <t>Panel: Building the Ecosystem: Investment, Alliances and Partnering – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>Chris Farmer, Founder &amp; CEO of SignalFire, is a successful serial entrepreneur and has extensive experience as a Partner in the VC industry, having run the seed fund at General Catalyst Partners. SignalFire is a complete redesign of the modern venture firm that brings unparalleled firepower at the seed stage to solve the biggest entrepreneur pain points. SignalFire uses a distributed network approach to provide expert advice from some of the world’s best entrepreneurs, product &amp; engineering leaders combined with cutting edge data infrastructure to help companies with recruiting exceptional talent, business development &amp; customer acquisition.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Chris-Farmer.jpg</t>
+  </si>
+  <si>
+    <t>Tim Chang is a proven investor (notable companies include Basis, ngMoco and Playdom), who invests in digitized health, community-based commerce, the sharing economy, brand analytics and virtual reality. He is passionate about the Future of Work, Health and Ecommerce and a frequent speaker on those topics at F.ounders, SXSW, Rutberg Mobile and other conferences. He currently works with the founders of Healthtap, Lantern, Massdrop, Moat, among others. He is a graduate of Stanford’s Business School and the University of Michigan, and an accomplished musician.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Tim-Chang.jpg</t>
+  </si>
+  <si>
+    <t>Patrick is the Managing Director of Qualcomm Ventures North America and leads all U.S. investments. He also serves as the Bay Area lead for Qualcomm Ventures and heads the Global Early Stage Fund, focused on Seed and Series A opportunities for the group. This fund has scaled to 60+ global investments over the past few years. While he works closely with nearly all the early stage portfolio companies around the world, he actively sourced or serves as a Board Member/Observer for investments in August, Blippar, Clarifai, Matterport, Navdy, OpenSignal, Skycatch, Sense360, Starmaker, Swift Nav and Zoom. Additionally he works very close with RetailNext, Tabtale and previously Waze (acquired by GOOG). Prior investments (exits) include Aicent, Divide (acquired by GOOG) Clicker (acquired by CBS), Tempo.AI (acquired by CRM), ThinkNear (acquired by TNAV) and Viewdle (acquired by GOOG). He also serves as the key investment lead on QPrize and Qualcomm Robotics Accelerator.
+Prior to joining Qualcomm Ventures, Patrick worked for Salomon Smith Barney’s Investment Banking unit in their Chicago, London and Hong Kong offices. He was a member of their Global Telecommunications team, involved in both M&amp;A advisory roles and capital-raising transactions. Patrick has an M.B.A. from the Kellogg Graduate School of Management and a B.A. from Northwestern University.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/Patrick-Eggen-photo.jpg</t>
+  </si>
+  <si>
+    <t>Robin Bordoli</t>
+  </si>
+  <si>
+    <t>CrowdFlower</t>
+  </si>
+  <si>
+    <t>Robin is Chief Executive Officer at CrowdFlower having joined the company in February 2015. Robin has spent the past two decades helping high growth companies launch and scale platforms and products into rapidly transforming markets.
+Prior to CrowdFlower, Robin was the Vice President &amp; General Manager, Strategic Consumer Industries at Marketo where he launched and led the business unit selling to consumer digital marketing teams. Robin has also held leadership roles at Jive Software, Worksimple, Yahoo, Excite@Home &amp; Micromuse.
+Robin holds a Master’s degree in Engineering from Cambridge University and a Master’s degree in Business Administration from Stanford University. Outside of work Robin spends his time trying to keep up with his two young children and enjoying all that the Bay Area has to offer</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/Robin-Bordoli-website.jpg</t>
+  </si>
+  <si>
+    <t>The 7 Myths of AI – Conference Luncheon</t>
+  </si>
+  <si>
+    <t>Boyd Davis</t>
+  </si>
+  <si>
+    <t>CEO &amp; Co-Founder</t>
+  </si>
+  <si>
+    <t>Kogentix</t>
+  </si>
+  <si>
+    <t>Boyd Davis is Chief Executive Officer and a co-founder of Kogentix. Davis launched Kogentix with his three co-founders based on their shared belief in the power of artificial intelligence fueled by open-source big data technology. By pulling together an organization of world class talent and delivering practical enterprise solutions with measurable results, the Kogentix executive team has overseen a rapid expansion of their business. Prior to founding Kogentix, Davis was Chief Operating Officer of Cask Data, a Palo Alto based venture-backed startup responsible for the leading application platform for Apache Hadoop. Davis started his career at Intel Corporation, where he worked for over two decades in a variety of sales, marketing, and general management positions. His last role at Intel was Vice President and General Manager of the Datacenter Software Division, a group which he formed to expand Intel’s business model beyond silicon into software. In that software division, he launched Intel’s distribution of Apache Hadoop and created a market leading position for Intel Hadoop in China. Those efforts ultimately led to Intel’s strategic investment in Cloudera to further optimize and accelerate adoption of Hadoop globally. Mr. Davis led the transition of the Hadoop business to Cloudera prior to his departure from Intel. Davis graduated from Purdue University with a Bachelor of Science in Electrical Engineering in 1990, and he resides in Portland, OR with his wife of 25 years and his three teenage children.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Boyd-Davis.jpg</t>
+  </si>
+  <si>
+    <t>Keynote: Practical AI Fueled by Big Data</t>
+  </si>
+  <si>
+    <t>Dr. Radhika Dirks</t>
+  </si>
+  <si>
+    <t>CEO &amp; Founder</t>
+  </si>
+  <si>
+    <t>Seldn</t>
+  </si>
+  <si>
+    <t>Head of Ventures North America</t>
+  </si>
+  <si>
+    <t>Radhika was recently nominated as one of Founders Fund’s 50 people changing the world through tech. She is currently the CEO &amp; Founder of a stealth startup Seldn – an artificial intelligence (AI) focused on predicting global macro risks. Seldn’s first product is a predictive risk integrated supply chain software.  Radhika is addicted to polymathy and fuses diverse expertise from various fields – from complexity physics &amp; quantum computing to finance &amp; global issues – to takes on Big Data, machine learning &amp; predictive analysis thru building an augmented next-gen enterprise software. She frequently advises, provides technical and commercialization expertise to several quantum computing groups.
+Previously, Radhika has built the world’s best source of entangled photons for quantum computing, co-led a Bio fuels spin out, and led due diligence on Future Energy deals as a founding member of Shell’s venture capital group. She’s also the founding COO of Rotary Gallop, a Big Data Finance Firm leveraging game theory to disrupt corporate control. Radhika has a PhD in quantum computing from the University of Illinois Urbana Champaign, where her thesis featured a whole chapter on teleportation.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/radhika263x273fin.jpg</t>
+  </si>
+  <si>
+    <t>Nigel Duffy</t>
+  </si>
+  <si>
+    <t>CTO</t>
+  </si>
+  <si>
+    <t>Sentient</t>
+  </si>
+  <si>
+    <t>Nigel Duffy leads the research, development, and commercialization of Sentient’s Artificial Intelligence technologies. A recognized expert in machine learning, Nigel was previously the co-founder and CTO at Numerate Inc. where he led technology development and managed the application of Numerate’s platform in collaborations with academics, biotechs, large pharmaceuticals companies, and the U.S. Government. Nigel invented Numerate’s core technologies which rapidly and repeatedly designed novel drug candidates for diseases including cancer, HCV, HIV, and heart disease. Prior to Numerate, Nigel was VP of Engineering at Pharmix and worked as a research scientist at AiLive (developer of the Wii Motion Plus), where he played a key role in applying machine learning to computer games. Nigel also spent time at Amazon A9 working on tools for large scale analytics in product search.
+The author of eleven granted or pending patents, Nigel’s technology is in regular use by more than 50 million users. He has published 15 academic papers including highly cited papers on machine learning, computational biology, and linguistics. Nigel holds a Masters in Mathematics from University College Dublin in Ireland and a PhD in Computer Science (Machine Learning Theory) from the University of California at Santa Cruz.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_nigelduffy.jpg</t>
+  </si>
+  <si>
+    <t>Keynote: The future of AI: More, better, faster decisions</t>
+  </si>
+  <si>
+    <t>Yoon C. Lee</t>
+  </si>
+  <si>
+    <t>Senior Vice President</t>
+  </si>
+  <si>
+    <t>Samsung Electronics America</t>
+  </si>
+  <si>
+    <t>Yoon C. Lee is Senior Vice President at Samsung Electronics America</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/Yoon-CLee-263x273.jpg</t>
+  </si>
+  <si>
+    <t>Mike Olson</t>
+  </si>
+  <si>
+    <t>Co-founder &amp; Chief Strategy Officer</t>
+  </si>
+  <si>
+    <t>Cloudera</t>
+  </si>
+  <si>
+    <t>Mike (@mikeolson) co-founded Cloudera in 2008 and served as its CEO until 2013 when he took on his current role of chief strategy officer (CSO.) As CSO, Mike is responsible for Cloudera’s product strategy, open source leadership, engineering alignment and direct engagement with customers. Prior to Cloudera Mike was CEO of Sleepycat Software, makers of Berkeley DB, the open source embedded database engine. Mike spent two years at Oracle Corporation as vice president for Embedded Technologies after Oracle’s acquisition of Sleepycat in 2006. Prior to joining Sleepycat, Mike held technical and business positions at database vendors Britton Lee, Illustra Information Technologies and Informix Software. Mike has a Bachelor’s and a Master’s Degree in Computer Science from the University of California, Berkeley.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/mikeolsen-263-273.jpg</t>
+  </si>
+  <si>
+    <t>Lawrence Flynn</t>
+  </si>
+  <si>
+    <t>Lawrence Flynn is a successful entrepreneur with over 20 years experience in managing international companies within the IT industry.
+At Artificial Solutions his focus on strategy and innovation, and his ability to re-engineer the organization to suit market circumstances and drive growth has placed the company at the forefront of the natural language revolution.
+Prior to joining Artificial Solutions, Lawrence’s foresight and shrewd business acumen resulted in several profitable trade exits for companies, over a wide range of sectors including ERP, Supply Chain and Web Content Management. In his previous role as CEO of MediaSurface, he floated the company on the London Stock Exchange and subsequently sold the company to Alterian, having grown revenues fivefold.
+Lawrence joined Artificial Solutions in May 2010 as CEO and has been instrumental in positioning the company as a leading player in the AI sector.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Lawrence-Flynn.jpg</t>
+  </si>
+  <si>
+    <t>Keynote: If Trees Could Walk – Open to all attendees</t>
+  </si>
+  <si>
+    <t>Dr. Catherine Havasi</t>
+  </si>
+  <si>
+    <t>Luminoso Technologies</t>
+  </si>
+  <si>
+    <t>Dr. Catherine Havasi is the CEO and Co-Founder of Luminoso Technologies, an Artificial Intelligence (AI)-based Deep Analytics Company in Cambridge, MA. Luminoso was founded on nearly a decade of research at the MIT Media Lab on how NLP and machine learning could be applied to text analytics. For over 15 years she has been researching language and learning and was a research scientist in artificial intelligence and computational linguistics at the MIT Media Lab where she ran the Digital Intuition group. In the late 90s, she co-founded the Common Sense Computing Initiative, or ConceptNet, a big-data lexical resource used in over two thousand academic projects.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/Dr.-Catherine-Havasi-website.jpg</t>
+  </si>
+  <si>
+    <t>Keynote: Illuminate Unknown Insights within your Data</t>
+  </si>
+  <si>
+    <t>Ashish Lahoti</t>
+  </si>
+  <si>
+    <t>SVP, Data &amp; Shared App Platforms</t>
+  </si>
+  <si>
+    <t>Wells Fargo</t>
+  </si>
+  <si>
+    <t>Ashish is a transformational leader, with 15 years of successfully leading turnarounds and launching greenfield platforms across Fortune 50 and start-up companies. He has led large-scale paradigm shifts to service oriented architecture (SOA), common business ontology, data self-service and platform as a service (PaaS) for democratized innovation across multi-billion dollar businesses, while simultaneously driving high levels of data consistency &amp; business agility.
+He heads data management and app development on enterprise platforms for hundreds of applications, web services, data and business analytic solutions, where he leads the implementation of high value solutions using Data Visualization, Machine Learning, and Big Data technologies for Consumer Lending Group.
+Previously, Ashish served in business and technical roles at IBM, Ford, Motorola and ICG Commerce, a B2B start-up acquired by Accenture.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/ashish-lahoti263x273fin.jpg</t>
+  </si>
+  <si>
+    <t>Bill Loconzolo</t>
+  </si>
+  <si>
+    <t>Vice President, Data Engineering</t>
+  </si>
+  <si>
+    <t>Intuit</t>
+  </si>
+  <si>
+    <t>Bill Loconzolo is the vice president of Intuit’s Data Engineering and Analytics team, where he leads the development of Intuit’s central big data platform, which leverages the power of the collective data of 37 million Intuit customers. The platform creates unique data-driven insights and product experiences that help customers simplify the business of life.
+Before joining the data team, Bill was the vice president of product development for Intuit’s Health division, which was focused on using data to change the way patients interact with their physicians, providers, and health plans. Bill joined Intuit in 2009 with the acquisition of Medfusion, where he served as CTO. Prior to Medfusion, he held multiple technology leadership positions, including CTO at Performix Technologies, senior architect at Nokia, and vice president of engineering at TeleGea.
+Bill has a BS in electrical engineering from Northeastern University. He is a frequent speaker at industry events and has published several software architecture papers. Currently, Bill holds a US patent on image processing and has US patents pending in the areas of VoIP services, data mart transformations, and performance-management business process reconciliation.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/Bill-Loconzolo-website.png</t>
+  </si>
+  <si>
+    <t>Executive Panel: AI Innovation in the Enterprise</t>
+  </si>
+  <si>
+    <t>President, Info &amp; Computer Sciences</t>
+  </si>
+  <si>
+    <t>SRI</t>
+  </si>
+  <si>
+    <t>Dr. William Mark is President of SRI International’s Information and Computing Sciences Division, which creates new technology in information security, system design, speech and natural language, vision and perception, planning and reasoning, and formal methods. The group’s leading-edge research is complemented with a strong focus on intellectual property creation and commercialization. Projects include Internet interaction, intrusion detection software, physical and virtual information spaces, and technology for dynamic enterprise management.
+Prior to joining SRI in 1998, Mark headed the System Technology Group at National Semiconductor. The group focused on system-level design and implementation of the silicon-based systems of the future, including hardware/software co-design, integrated DSP solutions, and reconfigurable computing technology.
+Mark was formerly director of Information and Computing Sciences for the Lockheed Martin Palo Alto Research Laboratories. Before joining Lockheed, he was a co-founder of Savoir, a company developing software tools for flexible manufacturing. He was a designer of the Flexis product, for which he holds a software patent. Previously, he held positions at the University of Southern California Information Sciences Institute and the General Motors Research Laboratories.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_williammark.jpg</t>
+  </si>
+  <si>
+    <t>Global &amp; US Data and Analytics Consulting Leader</t>
+  </si>
+  <si>
+    <t>PwC</t>
+  </si>
+  <si>
+    <t>Paul Blase is Global &amp; US Data and Analytics Consulting Leader at PwC, with 18 years of consulting experience working with senior executives from across industries on Strategy &amp; Business Design, Information &amp; Analytics and Mobilization/Execution opportunities and challenges related to improving their growth and margin. Paul currently leads PwC’s Data and Analytics Consulting team, with the mission of helping companies leverage advanced analytic and data capabilities to create an advantage in their business. In that role, Paul oversees an Innovation team that focuses on new big data and analytics techniques, including artificial intelligence and machine learning. Paul’s primary industry experience includes: Financial Services, Insurance, Healthcare, High Technology, and Travel &amp; Transportation.
+Paul has served as a senior advisory partner and lead engagement partner at companies including Life Technologies, Allstate, The Hartford, American Express, ACE, Intuit, PayPal, Citi, Travelers, Southwest Airlines, United Airlines, Avon, DLL, Equifax, Coca-Cola and Heidrick &amp; Struggles.
+At Diamond Management &amp; Technology Consultants, Paul was a member of the Management Committee where his leadership roles included co-leading the Insurance practice, leading the Enterprise Practice and co-leading cross-industry Service Lines.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/Paul-Blase-website.jpg</t>
+  </si>
+  <si>
+    <t>Keynote: Mind &amp; Machine: How AI helps business executives make better, faster strategic and operational decisions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Blase </t>
+  </si>
+  <si>
+    <t>Tolga Kurtoglu</t>
+  </si>
+  <si>
+    <t>VP, Director of System Sciences Lab (SSL)</t>
+  </si>
+  <si>
+    <t>Parc</t>
+  </si>
+  <si>
+    <t>Tolga Kurtoglu is Vice President and Director of the System Sciences Lab (SSL) at PARC. Research in SSL focuses on artificial intelligence, machine learning, control, planning, optimization, and high performance analytics for a variety of cyber-physical system applications serving Product Lifecycle Management (PLM), CAD/CAM, Transportation, Energy, and Aerospace and Defense sectors.
+Tolga leads the SSL team to create innovation and enterprise level business impact by applying leading edge scientific and technical solutions to solve complex real-world problems. He has served in various leadership roles at PARC focusing on product strategy and technology commercialization to manage transition of new technologies from an R&amp;D output to production quality software systems and services. Prior to his work with PARC, he worked as a researcher at NASA Ames Research Center and as a mechanical design engineer and group lead at Dell Corporation.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/Tolga-Kurtoglu.jpg</t>
+  </si>
+  <si>
+    <t>AI Case Studies: Pushing the Frontiers of Systems Engineering</t>
+  </si>
+  <si>
+    <t>Benjamin Levy</t>
+  </si>
+  <si>
+    <t>Co-Founder</t>
+  </si>
+  <si>
+    <t>BootstrapLabs</t>
+  </si>
+  <si>
+    <t>AI eats Software believer, Tech Investor, Startup Builder, Biz Dev, Funding, M&amp;A Expert, Windsurfer, Snowboarder, Husband &amp; Father.
+Ben is a Co-Founder of BootstrapLabs, a Venture Building Company that invests capital, experience and skills into disruptive AI software companies and helps their founders build global from Silicon Valley.
+Born in France and living in Silicon Valley for the past 17 years, Ben is a repeat entrepreneur who launched, built and exited two startups in the financial technology space. One was sold to Mergent and the other to SecondMarket, now part of NASDAQ.
+Ben helped founders raise over $300M of capital from Venture Capitalists and Private Equity Investors and closed $5B worth of technology M&amp;A transactions as an investment banker earlier in his career. He is also a frequent speaker on innovation, investing, technology, entrepreneurship and globalization in the US, Europe and Asia.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/Benjamin-Levy.jpg</t>
+  </si>
+  <si>
+    <t>David Linthicum</t>
+  </si>
+  <si>
+    <t>Sr. Vice President</t>
+  </si>
+  <si>
+    <t>Cloud Technology Partners</t>
+  </si>
+  <si>
+    <t>Leading technology publications frequently name David among the top 10 enterprise technologists in the world. He is a true thought leader in the industry, and an expert in complex distributed systems, including cloud computing, data integration, service oriented architecture (SOA), and big data systems. With more than 13 books on computing, more than 3,000 published articles, more than 500 conference presentations and numerous appearances on radio and TV programs, David has spent the last 20 years leading, showing and teaching businesses how to use resources more productively and innovate constantly. He has expanded the vision of both startups and established corporations as to what is possible and achievable.
+David’s industry experience includes tenures as CTO and CEO of several successful public and private software companies, and upper-level management positions in Fortune 100 companies. Dave has delivered over $2 billion dollars in value by transforming companies from traditional to innovative technologies, moving them to lucrative exits that benefitted investors, employees, and customers.
+Prior to joining Cloud Technology Partners, David founded Blue Mountain Labs, a cloud computing consulting and advisory firm (sold to Bick Ventures in Feb. 2010). David’s latest book is “Cloud Computing and SOA Convergence in Your Enterprise, a Step-by-Step Approach.”
+For more information about David, visit his personal site.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_davidlinthicum.jpg</t>
+  </si>
+  <si>
+    <t>Keynote: Cloud-Based Machine Learning…The Inside Story| Panel: Finding the Best Applications for AI and Machine Learning| AI Executive Summit</t>
+  </si>
+  <si>
+    <t>Dave Schubmehl</t>
+  </si>
+  <si>
+    <t>Research Director</t>
+  </si>
+  <si>
+    <t>IDC</t>
+  </si>
+  <si>
+    <t>Dave Schubmehl is Research Director for IDC’s Content Analytics, Discovery and Cognitive Systems research. His research covers information access and artificial intelligence technologies including content analytics, search systems, unstructured information representation, cognitive computing, deep learning, machine learning, unified access to structured and unstructured information, Big Data, visualization, and rich media search in SaaS, cloud and installed software environments.  This research analyzes the trends and dynamics of the content analytics, discovery and cognitive systems  software markets and the costs, benefits and workflow impacts of solutions that use these technologies.
+Mr. Schubmehl has over 25 years of experience working in the fields of enterprise search, information access and content analytics delivering products and services.  Prior to IDC, he was the Vice-President of Product Strategy for Janya, a provider of semantic analysis tools and solutions. Before Janya, he was the North American Account Manager for Fairview Research LLC, a consulting organization specializing in intellectual property and content analysis solutions.  He also served as the Vice-President and General Manager of the Discovery Products enterprise search business unit at Open Text Corporation. He has extensive experience in the development, marketing and sales of information access and search software as well as content and document management systems.  Prior to Open Text, Mr. Schubmehl was the Director of Development and Support for BRS Software Products and started his professional life as a software developer. Mr. Schubmehl attended the University at Albany.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/david-schubmehl.jpg</t>
+  </si>
+  <si>
+    <t>Jim McHugh</t>
+  </si>
+  <si>
+    <t>Vice President and General Manager</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>Jim leads the teams who are responsible for the NVIDIA DGX-1, the world’s first AI supercomputer in a box, and NVIDIA GRID, the leading solution for graphics virtualization. His responsibilities include product management, product marketing and partner solutions. Jim is focused on executing strategies to deliver GPU-based computing solutions for the data center.
+Jim has more than 25 years of experience as a marketing and business executive with many technology leaders including Apple, Cisco, and Sun. He has a deep understanding of business drivers, market/customer dynamics, and technology-centered products for AI, enterprise and data center applications.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/Jim-McHugh263x273.jpg</t>
+  </si>
+  <si>
+    <t>William Sobel</t>
+  </si>
+  <si>
+    <t>William Sobel has over 20 years of industry experience in successful startups managing the development of innovative application infrastructure software products. In recent years, as the principal author and architect of the MTConnect Standard, Mr. Sobel has led the industry toward significant advances in collection and analysis of machine data.
+Prior to System Insights, Mr. Sobel was VP/Chief Architect at MSCI-Barra, specializing in financial risk management software for some of the largest asset management companies in the world. Mr. Sobel led a team to architect and build their hosted risk management software as a service (SaaS) platform. In 1995, Mr. Sobel co-founded Redpoint Software, a leading capital markets enterprise risk management software company. At Redpoint, Mr. Sobel architected and built a real-time distributed database caching infrastructure to support fault tolerant parallelized analytics for financial risk management and trading systems.</t>
+  </si>
+  <si>
+    <t>Chief Strategy Officer</t>
+  </si>
+  <si>
+    <t>System Insights Inc.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/wsobel.jpg</t>
+  </si>
+  <si>
+    <t>Donald Thompson</t>
+  </si>
+  <si>
+    <t>Founder, President &amp; Chief Operating Officer</t>
+  </si>
+  <si>
+    <t>MAANA</t>
+  </si>
+  <si>
+    <t>As founder, President and Chief Operating Officer, Donald Thompson leads Maana’s product vision, oversees technology and product management, and is responsible for building and delivering cutting-edge solutions to Maana’s customers, some of the world’s largest corporations. With over 25 years of experience delivering high-profile, large-scale software and services, Donald has worked closely with top executives at Fortune 30 companies to develop and implement computing strategy across an array of industries, including oil and gas, health care, finance, retail, and travel. Prior to Maana, Donald spent 15 years at Microsoft as director of engineering, architect, and development manager within multiple divisions. He founded Bing’s Knowledge and Reasoning Team (project Satori); was co-founder of project Arena, which shipped as the SQL Server 2012 Semantic Engine; created Microsoft’s first contextual ad delivery system, spanning multiple international data centers to deliver over 14 billion targeted ads daily and generating $700MM annual revenue. Donald also oversaw numerous incubations in Microsoft Research and Windows.
+Prior to Microsoft, Donald was architect for a financial services startup, lead developer on a cellular billing system, and an independent consultant working on 3D graphics and physics engines for computer games.
+Donald earned a Master of Science in Computer Science from the University of Oxford. He has authored several technical publications and holds an array of patents covering data, wireless, search, and other technologies.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/Donald-Thompson-Filtered.jpg</t>
+  </si>
+  <si>
+    <t>Stephen Pratt</t>
+  </si>
+  <si>
+    <t>noodle.ai</t>
+  </si>
+  <si>
+    <t>Stephen is an instigator, agitator, and pioneer in creating world-class technology services organizations. He has spent his career building innovative ways to create value for the world’s most important organizations. Prior to Noodle, he was responsible for all Watson implementations worldwide for IBM Global Business Services. He also was the founder and CEO of Infosys Consulting, a Senior Partner at Deloitte Consulting, and a technology and strategy consultant at Booz, Allen &amp; Hamilton. He twice has been selected as one of the top 25 consultants in the world by Consulting Magazine. He has Bachelors and Masters degrees in Electrical Engineering from Northwestern University and The George Washington University focused on Satellite Communications.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_stephenpratt.jpg</t>
+  </si>
+  <si>
+    <t>Cristian Tanasescu</t>
+  </si>
+  <si>
+    <t>Executive Vice President</t>
+  </si>
+  <si>
+    <t>ESI Group</t>
+  </si>
+  <si>
+    <t>Cristian Tanasescu is Executive Vice-President at ESI Group and COO at Mineset Inc. In this role he is responsible for system modeling and big data analytics business unit.
+Previously, Cristian served as Vice President and General Manager Visual analytics at Silicon Graphics International (SGI) where he led the company initiative for a cloud-based data discovery and visualization application development. Cristian brings strong expertise in HPC, where he spent many years in leading the Software and Application Engineering organization at SGI.
+Prior to SGI, Cristian held engineering and management positions at Siemens, Fujitsu and Tecan AG.
+Cristian earned a M.S. in Computer Science from Polytechnic Institute of Bucharest, 1979.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Cristian-Tanasescu.jpg</t>
+  </si>
+  <si>
+    <t>Jordi Torras</t>
+  </si>
+  <si>
+    <t>CEO &amp; Fouender</t>
+  </si>
+  <si>
+    <t>Inbenta</t>
+  </si>
+  <si>
+    <t>Jordi Torras is the CEO and Founder of Inbenta, a company that specializes in Natural Language Processing, Machine Learning and Artificial Intelligence. Jordi founded Inbenta in 2005 to help companies improve online relationships with their customers through intelligent search, chatbots and a powerful e-commerce search appliance. Inbenta’s patented technology helps to greatly reduce incoming customer service emails, live chats and calls to call centers while increasing online conversions for industry-leading companies including Ticketmaster, CA Technologies and change.org.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/Jordi-Torras-website.jpg</t>
+  </si>
+  <si>
+    <t>Executive Panel: AI Innovation in the Enterprise| Seminar: Intelligent Assistants &amp; Bots</t>
+  </si>
+  <si>
+    <t>Eliot Weinman</t>
+  </si>
+  <si>
+    <t>Conference Chair, CEO</t>
+  </si>
+  <si>
+    <t>Trends Equity</t>
+  </si>
+  <si>
+    <t>Mr. Weinman is CEO/Founder of Trends Equity, Inc. and conference chair/founder of AI World. He is also executive editor of AI Trends. For over two decades, Eliot has been a successful entrepreneur and veteran high tech market expert. During this time, he has built and sold four leading publishing firms whose media, events and research services had become the largest in their respective industry.  Some of these include 4G World, RoboNexus, RoboBusiness Conference &amp; Expo, Mobile Commerce World and Application Development Conference &amp; Expo.  He has served as founding publisher, editor and author of numerous magazines, books and research studies in areas such as AI, mobile commerce, 4G/telecommunications, mobile internet, application development, IT, robotics and enterprise software. He has consulted to leading hardware, software and consulting firms, and his firms have partnered with and/or were acquired by companies such as Meta Group (now Gartner), IDG, CMP (now UBM), Yankee Group, Accenture, Internet.com, HP and others.
+Mr. Weinman is the editorial advisor to the San Francisco Chronicle “Future of Business and Technology” supplement where he authored the lead article “The A.I. World Awakens“. He is also editorial advisor for the November 2016 branded content section in FORTUNE (to be published Oct 26) on Cognitive Technologies. More information can be found here.  AI World and AI Trends were recently honored by FORTUNE who said,  “AI World and AI Trends are becoming the preeminent integrated media, publishing and conference brands in the industry.” click here for more info.
+Mr. Weinman received his M.S. in Computer Engineering from Boston University where he earned a research fellowship in AI thru a collaborative program with MIT and GE. After working at MIT’s Draper Lab’s in advanced software engineering and before starting his first publishing firm, he led the implementation one of the country’s first underwriting expert systems.  He served as chairman of the first U.S. conference on AI and expert systems for the financial services industry. Previously, he received his B.S. in Accounting and was a CPA for several large public accounting firms on Wall St.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/02/eliot-weinman.jpg</t>
+  </si>
+  <si>
+    <t>Industry Expert Wrap-Up| Conference Welcome</t>
+  </si>
+  <si>
+    <t>Oshiorenoya Agabi</t>
+  </si>
+  <si>
+    <t>Founder &amp; CEO</t>
+  </si>
+  <si>
+    <t>Koniku</t>
+  </si>
+  <si>
+    <t>Oshiorenoya Agabi (Founder &amp; CEO, Koniku Inc.), has over 10+ years of experience in neuroelectronic interfacing in industry and academia. As a strategic program lead at a robotics startup in Switzerland (Neuronics AG, acquired in 2008), Osh implemented learning algorithms for pick-and-place robots which worked alongside humans in a factory setting. The team achieved significant success in developing robots that learn object categorisation autonomously.
+Osh also led a cross disciplinary industry team to develop an in vitro reflex arc for modelling implantable neural chips. These chips interfaced with the peripheral nervous system. The project was completed with a successful design of an implantable chip lasting 30-40 years. He led applications of liquid state machines to biological neurons on chip, this was completed for the first time in 2004 at the ETH Zürich (Eidgenössische Technische Hochschule). He applied criteria for computability of biological neurons in vitro.
+As a visiting scholar and PhD candidate at the Imperial College in London, Osh built and customised 2 photon microscopes for studying synaptic transmission in the mouse visual cortex. He also worked on developing micro addressable spots for stimulating optogenetic neurons, a random access laser pixel for programming neurons in the mouse brain. This will help us better understand the mapping of visual signals from the thalamus to the visual cortex using a ‘thalamocortical’ slice in vitro. That is, “the various stages or relay stations of visual information processing in the brain.”</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/OSHI263x273.jpg</t>
+  </si>
+  <si>
+    <t>Panel: AI Disruption: Market Opportunities &amp; Threats</t>
+  </si>
+  <si>
+    <t>Amit Aghara</t>
+  </si>
+  <si>
+    <t>Global Head of Solution Management</t>
+  </si>
+  <si>
+    <t>KORE</t>
+  </si>
+  <si>
+    <t>AI Technology Solutions Theater – open to all attendees</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/AmitAghara263x2733.jpg</t>
+  </si>
+  <si>
+    <t>Modar Alaoui</t>
+  </si>
+  <si>
+    <t>Eyeris</t>
+  </si>
+  <si>
+    <t>Modar is a tech entrepreneur and expert in Artificially Intelligent vision technologies, Deep Learning and Ambient Intelligence. He is currently founder and CEO at Eyeris, the worldwide leading Deep Learning-based emotion recognition software. The company’s flagship product EmoVu reads facial micro-expressions in real-time and uses Convolutional Neural Networks (CNN’s) as a Deep Learning architecture to train and deploy its algorithm into a myriad of today’s commercial applications.
+Modar combines a decade of experience between Human Machine Interaction (HMI) and Audience Behavior Measurement. He is a frequent speaker and keynoter on “Ambient Intelligence” as the next frontier in AI, a winner of several technology and innovation awards and has been featured in the Wall Street Journal, the Huffington Post, Bloomberg and many other major publications for his work.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/Modar-Alaoui-262x272.jpg</t>
+  </si>
+  <si>
+    <t>Steve Ardire, is a software startup advisor with Artificial Intelligence, Machine Intelligence, and Cognitive Computing focus. Working with 40 startups over past 20 years, Steve shapes serendipity by interrogating reality to connect and illuminate the dots that matter to generate competitive business strategy with clarity, conviction, passion to drive business model to success.</t>
+  </si>
+  <si>
+    <t>Advisor to Software Startups</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_steveardire.jpg</t>
+  </si>
+  <si>
+    <t>Panel: AI Disruption: Market Opportunities &amp; Threats| Panel: Building the Ecosystem: Investment, Alliances and Partnering – Open to All Attendees| AI Startup Lightning Panel – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>Dalia Asterbadi</t>
+  </si>
+  <si>
+    <t>CEO &amp; Chief Data Scientist</t>
+  </si>
+  <si>
+    <t>verve.ai</t>
+  </si>
+  <si>
+    <t>Dalia Asterbadi, CEO of verve.ai, is a relentless problem solver. Her achievements came early. She led a team of marketers in one of Canada’s best managed companies at 24 and was a Director at a Publicly traded company at 25 – before co-founding (with her siblings) her first SaaS company, a communication and membership management system targeted at the non-profit sector.
+A systems engineer by trade, Dalia transitioned into sales and marketing, where she was a pioneer in data-driven marketing communications and sales analytics technology in early 2000. That has evolved into verve.ai, a customer experience augmented intelligence automation platform.
+Dalia has also published several papers on dynamic customer segmentation, funnel response and is author to several publications, including “The 31 Immutable Plays of Prospecting: The Truth Behind a Winning Culture and Bridging the Gap between Sales and Marketing”.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/Dalia-asterbadi-263x273.jpg</t>
+  </si>
+  <si>
+    <t>John Axerio-Cilies</t>
+  </si>
+  <si>
+    <t>CTO, Founder</t>
+  </si>
+  <si>
+    <t>Arterys Inc.</t>
+  </si>
+  <si>
+    <t>John Axerio-Cilies, CTO and co-founder of Arterys. As CTO, John leads the development of the first cloud platform to gather, process, analyze and report on medical images from anywhere in the world. He is also responsible for leading the company’s deep learning and regulatory teams. Prior to this role, John held various leadership, design and development positions at Blue Energy Canada, Honeywell, and Bosch. He holds a PhD in Engineering from Stanford University (Flow Physics and Computational Engineering), participated in the highly selective Stanford Graduate School of Business PRIE program, and has a Master’s degree in Aeronautics and Astronautics from Stanford University. He also was a 2011 StartX Fellow, one of the top 70 Stanford student entrepreneurs selected for this honor.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/John-Axerio.png</t>
+  </si>
+  <si>
+    <t>Panel: AI and Cognitive Computing in Healthcare</t>
+  </si>
+  <si>
+    <t>AI Technology Solutions Theater – open to all attendees| AI Startup Lightning Panel – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>Tom Baltis</t>
+  </si>
+  <si>
+    <t>VP, CISO</t>
+  </si>
+  <si>
+    <t>Blue Cross Blue Shield of Michigan</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/nophoto263x273.jpg</t>
+  </si>
+  <si>
+    <t>Award-winning executive Tom Baltis transforms cyber security into a powerful brand differentiator driving customer acquisition and retention. Mr. Baltis currently serves as Vice President and Chief Information Security Officer at Blue Cross Blue Shield of Michigan, the third largest Blue Cross Blue Shield plan. With 15 years of leadership experience, he has established and led world-class information security organizations at Fortune 100 companies in healthcare, financial services, defense, and other highly regulated industries. Very active in the startup community, Tom is sought out by top-tier venture capital firms to identify winning product ideas and future market disruptors. As a trusted advisor, he helps emerging and established technology companies raise capital, accelerate revenue growth, and achieve leading market share.
+Tom envisions cyber security as creating business value and competitive advantage. This vision is enabled by continuous innovation, most recently in portfolio management approaches to security investment, advanced threat detection powered by big data technologies, agile security methodologies, and real-time threat intelligence platforms. A frequent speaker at conferences and industry roundtables, he has been recognized internationally by business leaders, industry analysts and government regulators for promoting cross-sector collaboration in the fight against cyber crime, enabling business strategies through security innovation, and elevating cyber security to a brand-level issue.</t>
+  </si>
+  <si>
+    <t>Panel: Machine Learning and Security in the Enterprise</t>
+  </si>
+  <si>
+    <t>Michael Barnett</t>
+  </si>
+  <si>
+    <t>Founder/EVP</t>
+  </si>
+  <si>
+    <t>SmartCloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mike began his industrial AI career at Rice University, where his doctorate focused on dynamic modeling, simulation, and AI-based control. His 25 years of experience with AI includes working with Gensym, as well as consulting and research for Fortune 1000 clients in the energy and utility, manufacturing, supply chain, pharmaceutical, oil and gas, and water/wastewater industries.
+</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/mikebarnett.jpg</t>
+  </si>
+  <si>
+    <t>Panel: AI &amp; Real Time Intelligence for IoT</t>
+  </si>
+  <si>
+    <t>Chris Belmont</t>
+  </si>
+  <si>
+    <t>VP, CIO, MD</t>
+  </si>
+  <si>
+    <t>Anderson Cancer Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris Belmont is the Chief Information Officer at the University of Texas MD Anderson Cancer Center. Chris has over 30 years healthcare IT experience from various positions in IT leadership, sales and consulting with Siemens, Healthlink and IBM. Chris is now leading MD Anderson through a system wide Epic, EMR rollout.
+</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/speakers/chris-belmont/</t>
+  </si>
+  <si>
+    <t>Nick Brestoff</t>
+  </si>
+  <si>
+    <t>IntraSpexion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick Brestoff earned two degrees in engineering from UCLA and Caltech before he went to law school at USC, where he was a member of the Law Review. He specialized in litigation matters in state and federal court in California for 38 years before he left the profession in order to found Intraspexion. He is the principal author of Preventing Litigation: An Early Warning System to Get Big Value Out of Big Data (Business Expert Press 2015), which Sir Richard Susskind endorsed. His many articles on using technology in the legal profession have appeared in a variety of publications, e.g., the ABA’s Journal of Electronic Discovery and Digital Evidence, Law Technology News, and Corporate Counsel.
+</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/08/Nick-Brestoff.jpg</t>
+  </si>
+  <si>
+    <t>Andrea L. Cardozo</t>
+  </si>
+  <si>
+    <t>Head of Consumer Insights</t>
+  </si>
+  <si>
+    <t>Pandora Media</t>
+  </si>
+  <si>
+    <t>Andrea Lopus Cardozo is the head of Consumer Insights for the Brand and Product Marketing department at Pandora Media. She and her team conduct a variety of research in the U.S. and abroad including brand equity tracking, product concept testing and ad effectiveness tracking. Previously, she spent seven years in the Consumer Insights department at the Clorox Company supporting the International, Innovation and New Business teams. Andrea has an MBA in Marketing from the Wharton school at the University of Pennsylvania, an MA in International Studies from the University of Pennsylvania and a BA in Psychology from the University of California, Berkeley.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/AndreaCardozo-263x273.jpg</t>
+  </si>
+  <si>
+    <t>James Chan</t>
+  </si>
+  <si>
+    <t>Bloomberg Beta L.P</t>
+  </si>
+  <si>
+    <t>Juhi Chandalia</t>
+  </si>
+  <si>
+    <t>Senior Data Scientist</t>
+  </si>
+  <si>
+    <t>Sentient Technologies</t>
+  </si>
+  <si>
+    <t>Juhi Chandalia is a senior data scientist at Sentient Technologies, where she applies deep learning to data science problems. She focuses specifically on rapidly prototyping solutions for new business use cases. Before relocating to the Bay Area, she ran a data science consulting company in Boston. Juhi has degrees in physics (BS and MS) and electrical engineering (BS) from MIT. When she’s not doing data science, you can find her enjoying the outdoors, making art, or eating tasty food.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/Juhi-Chandalia-website.jpg</t>
+  </si>
+  <si>
+    <t>When Artificial Intelligence Meets Virtual Reality</t>
+  </si>
+  <si>
+    <t>Jerry Chen</t>
+  </si>
+  <si>
+    <t>Bus Dev, AI &amp; Industrial IoT</t>
+  </si>
+  <si>
+    <t>Jerry Chen is responsible for developing the partner ecosystem for artificial intelligence and machine learning at NVIDIA. Past roles include management positions in professional graphics, scientific HPC, and structural mechanics. He holds a Bachelors and Masters of Engineering from Cornell University and an MBA from the University of California at Berkeley.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/Jerry-Chen.jpg</t>
+  </si>
+  <si>
+    <t>Panel: High Performance Computing for the AI Ecosystem</t>
+  </si>
+  <si>
+    <t>Derek Collison</t>
+  </si>
+  <si>
+    <t>Apcera</t>
+  </si>
+  <si>
+    <t>Derek Collison is founder and CEO of Apcera. An industry veteran and pioneer in large-scale distributed systems and enterprise computing, Derek has held executive positions at VMware, Google and TIBCO Software.
+As CTO and chief architect of cloud application platforms at VMware, he cofounded the cloud computing group and designed and architected Cloud Foundry, the industry’s first open PaaS. During his time at Google, he co-founded the AJAX APIs group. Prior to Google, he spent more than a decade at TIBCO, where he designed and implemented a wide range of messaging products, including Rendezvous and EMS. As TIBCO’s senior vice president and chief architect, Derek led technical and strategic product direction and delivery.
+Derek is a sought after speaker and collaborator. He holds more than 20 software patents and is a recognized leader in distributed systems design and architecture, as well as emerging cloud platforms. He earned a bachelor’s degree with honors in Computer Science from the University of Maryland.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/Derek-Collison-262x272.jpg</t>
+  </si>
+  <si>
+    <t>Panel: Advances in Machine Learning</t>
+  </si>
+  <si>
+    <t>Tamara Carelton</t>
+  </si>
+  <si>
+    <t>Innovation Leadership Board LLC</t>
+  </si>
+  <si>
+    <t>Tamara Carleton, Ph.D., is CEO and founder of Innovation Leadership Board LLC, a global leader in the design of tools and processes that enable radical innovation. Previously, Dr. Carleton served as a Fellow at the U.S. Chamber of Commerce Foundation, as Fellow with the Foundation for Enterprise Development, and as Fellow for the Bay Area Science and Innovation Consortium. A former management consultant at Deloitte Consulting LLP, Dr. Carleton specialized in emerging solutions in enterprise applications, customer experience, and marketing strategy. She has been published in a variety of technical journals, as well as the general business press. Dr. Carleton is frequently invited to discuss her work and research in the United States and abroad.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/aiworld_speakers_tamaracarleton.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel: AI Disruption: Market Opportunities &amp; Threats  </t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/Adam-Devine-website.jpg</t>
+  </si>
+  <si>
+    <t>VP, Head of Marketing</t>
+  </si>
+  <si>
+    <t>WorkFusion</t>
+  </si>
+  <si>
+    <t>Adam Devine runs marketing for WorkFusion, AI-powered intelligent automation software for enterprise operations. He is accountable for product marketing, corporate communications, demand generation, and customer and partner education. Adam joined WorkFusion as its first marketer in 2012 and has helped to grow WorkFusion into the leading solution in intelligent automation. He began his career in management consulting at KPMG Consulting’s Banking &amp; Capital Markets practice, founded several companies, and held officer roles in strategic planning at some of the top advertising and branding agencies, including Droga5, 360i, and McCann Erickson. Adam has authored numerous business and technical papers and speaks frequently about robotics, cognitive automation, and machine learning at technology and BFSI industry conferences, including AI &amp; RPA World Summit, IRPA, FIMA, MarketTech, NAFIS, NASSCOM, and Strata+Hadoop World. Adam lives in Manhattan’s West Village but frequently escapes to ski, surf, and kiteboard.</t>
+  </si>
+  <si>
+    <t>Continental Breakfast – Hosted by WorkFusion| Panel: Finding the Best Applications for AI and Machine Learning| AI Technology Solutions Theater – open to all attendees</t>
+  </si>
+  <si>
+    <t>Gregory Diamos</t>
+  </si>
+  <si>
+    <t>Senior Researcher, Baidu, Inc.</t>
+  </si>
+  <si>
+    <t>Greg is Senior Researcher at Baidu, Inc. His current focus includes application of High Performance Computing technologies to training deep neural networks and attempting to achieve strong scaling of deep neural network training to 1000s of high throughput processors while maintaining a high level programming model. Interested in understanding the design space of high performance processor architectures and effective deep neural network architectures
+Previously he was with NVIDIA. He received his PhD from the Georgia Institute of Technology. At Georgia Tech he contributed to the development of the GPU-Ocelot dynamic compiler, which targeted CPUs and GPUs from the same program representation. His Ph.D. thesis pioneered execution models for heterogeneous processors.</t>
+  </si>
+  <si>
+    <t>Baidu, Inc.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/gregdiamos-263x273v1.jpg</t>
+  </si>
+  <si>
+    <t>Michael Dierickx</t>
+  </si>
+  <si>
+    <t>Information Security Officer</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>Mike is Information Security Officer at Panasonic. He is currently involved in and responsible for: Conducting penetration testing of commercial aircraft systems and automobiles, designing and implementation of security architecture of aircraft, automobiles, and backend ground systems, Panasonic North America PSIRT(Product Security Incident Response Team) Leader Implementing disaster recovery and business continuity planning for aircraft facing networks. He is involved in the Western Regional Collegiate Cyber Defense Competition – Red Team Member and at 2013 ISE West he was an Information Security Executive of the Year Nominee.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/MikeDierickx-263x273v3.jpg</t>
+  </si>
+  <si>
+    <t>Saman Farid</t>
+  </si>
+  <si>
+    <t>Comet Labs</t>
+  </si>
+  <si>
+    <t>Saman is a passionate supporter of early- stage startups. He has built three companies in the areas of e-commerce, IP television, and logistics management, and faced the challenges of building, focusing, and scaling a company. Two exits later, Saman is now working on building a new home for smart machines – Comet Labs, which invests in robotics companies and will enable robotics and AI companies to build better products, find customers, and scale faster.
+Saman has spent more than 15 years in China, and has held positions at Honeywell, Verizon, Deloitte Consulting and Microsoft in roles ranging from R&amp;D to operations optimization. He received his Bachelor’s degree in Control Systems Engineering from the Cooper Union and his MBA from Tsinghua and MIT.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/05/Saman-Farid-262x272.jpg</t>
+  </si>
+  <si>
+    <t>AI Startup Lightning Panel – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>Scott Fullman</t>
+  </si>
+  <si>
+    <t>Director, Analytics</t>
+  </si>
+  <si>
+    <t>Scott is a director in PwC’s Analytics Innovation group. He has eight years of consulting experience focused in data, analytics, and software development. Scott has led a number of domestic and international projects, ultimately working on four continents, and has played roles in both the business strategy and technical design aspects of developing new products.
+Scott currently leads PwC’s Analytics Innovation Accelerator group which is focused on using data analytics tools and techniques to create new products and differentiated service offerings for clients. Previous to running the Innovation program, Scott led the creation of PwC’s Supply Chain Risk Analytics product.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/Scott-Fullman-website.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel: AI Disruption: Market Opportunities &amp; Threats </t>
+  </si>
+  <si>
+    <t>Rethink Technology Research</t>
+  </si>
+  <si>
+    <t>Caroline is currently writing a special report with AI Trends entitled: AI: Commercial Impact in Vertical Markets
+Caroline co-founded Rethink Technology Research in 2002 to focus on emerging mobile technologies and their impact on operator business models. She has been analyzing and reporting in the hi-tech industries since 1986 and has a huge wealth of experience of technology trends and how they impact on business models. She started her career as a technology journalist and then took senior roles in online publishing and research before focusing full time on wireless industry research and consultancy.
+At Rethink her role has been to head up the wireless side of the business. This focuses on RAN and core network deployments and operators’ IT strategies and business cases. Rethink produces forecasts and analysis based on an opt-in research base of senior executives at over 100 mobile, converged and IoT operators.
+Caroline leads the creation of research, newsletters and consulting services focused on these operator models. In this role, she has become a highly recognized authority on 4G systems such as LTE, and carrier network strategies such as HetNet, and a prolific speaker at industry events.
+Prior to Rethink, Caroline held various executive positions at VNU Business Publishing, then the largest provider of technology publications and research in Europe. Among her roles were operations director of the pan-European online business, and European content director. She holds an MA from the University of Oxford.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/07/Caroline-Garbiel.jpg</t>
+  </si>
+  <si>
+    <t>Industry Expert Wrap-Up| Panel: AI &amp; Real Time Intelligence for IoT| Enteprise AI Adoption: A Study of Vertical Industry Adoption – Open to All Attendees</t>
+  </si>
+  <si>
+    <t>Anju Gupta</t>
+  </si>
+  <si>
+    <t>Director, Digital Partnerships &amp; Outreach</t>
+  </si>
+  <si>
+    <t>Monsanto</t>
+  </si>
+  <si>
+    <t>Anju Gupta currently leads the Global IT Strategic Collaborations at Monsanto. In this role, she is responsible for establishing high level strategic partnership ecosystem for Monsanto with industry partners. Anju joined Monsanto in 2003 as a Molecular Scientist and transitioned into leading Statistical Genetics and analytical teams. In the recent years, she focused on building long term strategies for Monsanto’s crop portfolio for US and Latin America North. She has been an active contributor to several non profit organizations. She has received numerous awards including few Monsanto Above and Beyond awards. She was also nominated as the YWCA Women leader for Monsanto in 2014. Anju has a Ph.D in Quantitative genetics from The Ohio State University and has ~17 granted and published patents.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/anju-gupta-263x273.jpg</t>
+  </si>
+  <si>
+    <t>Executive Roundtable: Evolution or Disruption?| Driving Deep Learning Adoption Within the Enterprise</t>
+  </si>
+  <si>
+    <t>Ilya Gelfenbeyn</t>
+  </si>
+  <si>
+    <t>Product Manager of API.AI</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Ilya Gelfenbeyn is the product manager for API.AI at Google. Ilya co-founded API.AI in 2010 and served as the company CEO. API.AI is a developer platform for building conversational experiences into products and services. Over 60k developers use API.AI to build chatbots, Prior to launching API.AI, the company built Assistant.ai, the highest rated independent voice assistant in the world with 40M+ users.
+Ilya earned his MBA from the University of Brighton, and a BSc in Mathematics from Novosibirsk State University. Ilya’s areas of interest are in natural language processing, artificial intelligence and conversational interfaces. He is an author of a number of patents in those fields.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/Ilya-Gelfenbeyn-webiste.jpg</t>
+  </si>
+  <si>
+    <t>Isabelle Guis</t>
+  </si>
+  <si>
+    <t>Isabelle Guis is the Chief Strategy Officer at Egnyte, overseeing all global marketing, go-to-market, partnership and product strategies. She previously served as EMC’s vice president of Marketing for the Public Cloud Solutions Group and Enterprise Storage Division, driving cloud buyer and service provider segmentations, as well as messaging, product positioning and go-to-market strategies for the company’s core storage solutions. Isabelle has also held leadership positions at Avaya, Big Switch Networks, Cisco Systems, and Nortel Networks. She holds a Master of Science in Electrical Engineering and Computer Science from Supelec (France), and an MBA from Harvard Business School.</t>
+  </si>
+  <si>
+    <t>Egnyte</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/isabelle-Guis-273x263-262x263.jpg</t>
+  </si>
+  <si>
+    <t>Daniel Gutierrez</t>
+  </si>
+  <si>
+    <t>Managing Editor</t>
+  </si>
+  <si>
+    <t>InsideBIGDATA</t>
+  </si>
+  <si>
+    <t>Daniel D. Gutierrez is a data scientist with Los Angeles-based AMULET Analytics. He’s been involved with data science and Big Data long before the fields came in vogue, so imagine his delight when the Harvard Business Review deemed “data scientist” as the sexiest profession for the 21st century! As a Big Data journalist, he enjoys keeping a pulse on this fast-paced industry. He’s also an educator having taught data science, machine learning and R classes for UCLA, UC Irvine, and UC Davis. He’s authored four computer industry books on database and data science technology, including his most recent title, “Machine Learning and Data Science: An Introduction to Statistical Learning Methods with R.” Daniel sits on a number of advisory boards to bring the benefits of data science to businesses.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/DanGutierrez263x273v1-262x272.jpg</t>
+  </si>
+  <si>
+    <t>Babak Hodjat</t>
+  </si>
+  <si>
+    <t>Co-Founder &amp; Chief Scientist</t>
+  </si>
+  <si>
+    <t>Babak Hodjat is co-founder and chief scientist of Sentient, responsible for the core technology behind the world’s largest distributed artificial intelligence system. Babak is a serial entrepreneur, having started a number of Silicon Valley companies as main inventor and technologist. Prior to co-founding Sentient, Babak was senior director of engineering at Sybase iAnywhere, where he led mobile solutions engineering. Prior to Sybase, Babak was co-founder, CTO and board member of Dejima Inc., acquired by Sybase in April 2004. Babak is the primary inventor of Dejima’s patented, agent-oriented technology applied to intelligent interfaces for mobile and enterprise computing – the technology behind Apple’s Siri. Babak is a published scholar in the fields of Artificial Life, Agent-Oriented Software Engineering, and Distributed Artificial Intelligence, and has 25 granted or pending patents to his name.
+Babak holds a PhD in Machine Intelligence from Kyushu University, in Fukuoka, Japan.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/babak-hodjat-263-273v1.jpg</t>
+  </si>
+  <si>
+    <t>Fireside Chat with Babak Hodjat, Co-Founder/Chief Scientist, Sentient – Open to all Attendees</t>
+  </si>
+  <si>
+    <t>Amir Husain</t>
+  </si>
+  <si>
+    <t>SparkCognition</t>
+  </si>
+  <si>
+    <t>Amir Husain, recognized as Austin’s Top Technology Entrepreneur of 2015 by the Austin Business Journal, and awarded the Austin Under 40 Technology and Science Award, is a serial entrepreneur and inventor based in Austin, Texas. He is the Founder &amp; CEO of SparkCognition, Inc. an award-winning Machine Learning/AI driven Cognitive Analytics Company, a Member of the Board of Advisors for IBM Watson, and a Member of the Board of Advisors for The University of Texas at Austin, Dept. of Computer Science.
+Amir is a prolific inventor with 14 awarded and over 40 pending US patent applications to his credit. In 2013, a low cost computing platform Amir invented was inducted into the collection of the Computer History Museum in Mountain View, the world’s largest such institution. His work has also been published in IEEE conferences and in leading tech journals including Network World, Computer World and others. His companies have won numerous awards such as the 2015 Austin Chamber of Commerce A-List, Nokia’s 2015 Open Innovation Challenge, the InnovateApp 2014 competition, the VMWORLD Gold award, Network World’s Hottest Products, CRN’s Innovation award and PC World’s best product award. Amir also serves as advisor and board member to Makerarm, uStudio, AM Networks, Pepper.pk, S&amp;BMK Foundation, Alif Laila Children’s Educational Society, and others.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/06/Amir-Husain.jpg</t>
+  </si>
+  <si>
+    <t>Dr. Sindhu Joseph</t>
+  </si>
+  <si>
+    <t>CogniCor</t>
+  </si>
+  <si>
+    <t>Dr. Joseph is an entrepreneur, with  has a doctorate degree in Artificial Intelligence and  an inventor of 6 US patents in artificial intelligence. CogniCor was born out of her PhD thesis and her personal experiences with a problem that most people face – The need for good Customer service that really solves issues.  CogniCor is the award winning provider of automated customer service technology for large enterprises. CogniCor’s patent pending artificial intelligence based technology enables enterprises to solve customer queries and issues instantly, minimizing human intervention while enabling corporates to have  significant opex savings and customers to get instant personalized resolution to their queries.  Some of the top Telcos in Europe and banks in Asia use CogniCor  platform for digital customer care.
+Since co-founding CogniCor, along with Rosh Cherian,  and establishing a globally distributed and talented team, she was instrumental in raising a seed round of 1M with international investors. CogniCor was named as the most innovative web startup from Europe by European commission, and chosen by British Telecom for the   “delighting tomorrow’s customers” award and is also winner of the best emerging start up from NASSCOM India. The printed edition of WIRED magazine, selected  as one of the hottest startups from Europe.
+While current technologies adopt a deterministic method of resolving customer issues, CogniCor’s cognitive resolution agent platform (CIRA) blends state of the art technologies in Natural language processing, data analytics and machine learning to create an artificial intelligence enabled virtual resolution agent that works autonomously for self service as well as assists real agents for resolving issues and “learns” from previous resolutions by a human.
+Born in a small town in southern India, and educated in India and Europe, Sindhu was selected as one of the most outstanding entrepreneurs from the UK,  a finalist in Google Anita Borg award, and worked for Honeywell Research prior to her PhD. A visionary leader and inventor and  a mother of two kids, she hopes to be a role model for women in technology and has inspired many in her home country to adopt career in business and technology.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/09/SindhuJoseph-263x273v1.jpg</t>
+  </si>
+  <si>
+    <t>Dan Kara</t>
+  </si>
+  <si>
+    <t>Research Director, Robotics</t>
+  </si>
+  <si>
+    <t>ABI Research</t>
+  </si>
+  <si>
+    <t>Dan Kara is Practice Director, Robotics, Automation and Intelligent Systems at ABI Research, a technology market intelligence company with a 25 year track record of putting information into the hands of executives in order to enable them to make the right decisions on technology and market investment. Prior to joining ABI, Dan was Chief Research Officer for Myria RAS, a research and advisory services firm focused on automation, robotics and intelligent systems trends, and publisher of the ARISPlex.com robotics portal. Dan was also President of Robotics Trends, an integrated media and research firm serving the personal, service and mobile robotics markets. Dan has also worked as Executive Vice President of Intermedia Group and Director of Research at Ullo International.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/04/Kara_HiRez-262x272.jpg</t>
+  </si>
+  <si>
+    <t>Smart Robotics: Making Robots Intelligent, Cognitive &amp; Aware| Industry Expert Wrap-Up</t>
+  </si>
+  <si>
+    <t>Rahul Kelkar</t>
+  </si>
+  <si>
+    <t>Lead Architect</t>
+  </si>
+  <si>
+    <t>ignio</t>
+  </si>
+  <si>
+    <t>Rahul Kelkar holds the position of Principal Scientist and Head of Incubation at Digitate, a Tata Consultancy Services venture. In his role, Rahul serves as the Chief Architect for ignio™, the flagship offering from Digitate. He brings to this position more than twenty years of deep IT experience working as a transformation architect for large IT transformation programs. Rahul holds a Master’s degree in mechanical engineering, with an emphasis on design engineering. His professional areas of interest span software testing, grid computing, software streaming, autonomous computing, automation, and analytics.
+Prior to joining TCS and Digitate, Rahul worked with Fujitsu-Siemens Computer, Inc. He holds the following patents: for converting procedural text to an actionable knowledge form; for systems and methods for generating and implementing monitoring solutions for a computing-based infrastructure; and for system and method for configuring and executing services. Rahul’s published articles include: Run-time Dependency Tracking in Data Centers; Knowledge Acquisition for Automation in IT Support; Opportunities in System Testing; eTransform: Transforming Enterprise Data Centers by Automation Consolidation; and Towards Automating the Security Compliance Value Chain.</t>
+  </si>
+  <si>
+    <t>http://aiworldexpo.com/wp-content/uploads/2016/10/Rahul-Kelkar-website-262x272.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,6 +1759,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="6"/>
+      <color rgb="FF595959"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -734,9 +1796,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -745,6 +1804,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1062,7 +2122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1081,16 +2141,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -1099,25 +2159,25 @@
         <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B2" s="3">
         <v>0.54166666666666663</v>
@@ -1132,23 +2192,23 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3">
@@ -1161,21 +2221,21 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B4" s="3">
         <v>0.54166666666666663</v>
@@ -1184,24 +2244,24 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B5" s="3">
         <v>0.54166666666666663</v>
@@ -1210,19 +2270,19 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1230,7 +2290,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B6" s="3">
         <v>0.54861111111111105</v>
@@ -1239,19 +2299,19 @@
         <v>0.56597222222222221</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I6" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1259,7 +2319,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3">
         <v>0.56597222222222221</v>
@@ -1268,22 +2328,22 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -1291,7 +2351,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B8" s="3">
         <v>0.58333333333333337</v>
@@ -1300,19 +2360,19 @@
         <v>0.59722222222222221</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H8" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I8" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -1320,7 +2380,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B9" s="3">
         <v>0.59722222222222221</v>
@@ -1329,19 +2389,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
         <v>116</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H9" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" t="s">
-        <v>126</v>
       </c>
       <c r="L9">
         <v>5</v>
@@ -1349,7 +2409,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B10" s="3">
         <v>0.61111111111111105</v>
@@ -1359,13 +2419,13 @@
       </c>
       <c r="D10" s="3"/>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="L10">
         <v>6</v>
@@ -1373,7 +2433,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B11" s="3">
         <v>0.625</v>
@@ -1382,22 +2442,22 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H11" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L11">
         <v>7</v>
@@ -1405,7 +2465,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B12" s="3">
         <v>0.64583333333333337</v>
@@ -1414,19 +2474,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="F12" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H12" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="L12">
         <v>8</v>
@@ -1434,7 +2494,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B13" s="3">
         <v>0.66666666666666663</v>
@@ -1443,19 +2503,19 @@
         <v>0.69791666666666663</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H13" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I13" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="L13">
         <v>9</v>
@@ -1463,7 +2523,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3">
         <v>0.61458333333333337</v>
@@ -1472,18 +2532,18 @@
         <v>0.63541666666666663</v>
       </c>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3">
         <v>0.70833333333333337</v>
@@ -1492,27 +2552,27 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B16" s="3">
         <v>0.75</v>
@@ -1521,30 +2581,30 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F16" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G16" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J16" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B17" s="3">
         <v>0.77083333333333337</v>
@@ -1553,33 +2613,33 @@
         <v>0.8125</v>
       </c>
       <c r="D17" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+      <c r="F17" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" t="s">
         <v>139</v>
       </c>
-      <c r="E17" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" t="s">
-        <v>125</v>
-      </c>
-      <c r="G17" t="s">
-        <v>149</v>
-      </c>
       <c r="H17" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="J17" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="K17" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B18" s="3">
         <v>0.77083333333333337</v>
@@ -1588,22 +2648,22 @@
         <v>0.8125</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="G18" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1635,16 +2695,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
@@ -1653,25 +2713,25 @@
         <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B2" s="3">
         <v>0.34375</v>
@@ -1680,27 +2740,27 @@
         <v>0.36458333333333331</v>
       </c>
       <c r="D2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="G2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3">
         <v>0.375</v>
@@ -1709,27 +2769,27 @@
         <v>0.38194444444444442</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="F3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B4" s="3">
         <v>0.38194444444444442</v>
@@ -1738,30 +2798,30 @@
         <v>0.40625</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B5" s="3">
         <v>0.40625</v>
@@ -1770,27 +2830,27 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="F5" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B6" s="3">
         <v>0.42708333333333331</v>
@@ -1799,15 +2859,15 @@
         <v>0.4375</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B7" s="3">
         <v>0.4375</v>
@@ -1816,27 +2876,27 @@
         <v>0.4548611111111111</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G7" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I7" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B8" s="3">
         <v>0.4548611111111111</v>
@@ -1845,24 +2905,24 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="E8" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G8" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="J8" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B9" s="3">
         <v>0.47916666666666669</v>
@@ -1871,24 +2931,24 @@
         <v>0.49305555555555558</v>
       </c>
       <c r="E9" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="H9" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B10" s="3">
         <v>0.49305555555555558</v>
@@ -1897,27 +2957,27 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G10" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="H10" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I10" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B11" s="3">
         <v>0.51041666666666663</v>
@@ -1926,21 +2986,21 @@
         <v>0.5625</v>
       </c>
       <c r="D11" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="F11" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B12" s="3">
         <v>0.5625</v>
@@ -1949,27 +3009,27 @@
         <v>0.59375</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E12" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H12" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I12" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J12" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B13" s="3">
         <v>0.5625</v>
@@ -1978,30 +3038,30 @@
         <v>0.59375</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E13" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F13" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G13" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="H13" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="J13" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B14" s="3">
         <v>0.5625</v>
@@ -2010,27 +3070,27 @@
         <v>0.59375</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E14" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="F14" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="G14" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B15" s="3">
         <v>0.59375</v>
@@ -2039,27 +3099,27 @@
         <v>0.625</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="E15" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="G15" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="J15" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B16" s="3">
         <v>0.59375</v>
@@ -2068,30 +3128,30 @@
         <v>0.625</v>
       </c>
       <c r="D16" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E16" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="F16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16" t="s">
         <v>198</v>
       </c>
-      <c r="G16" t="s">
-        <v>208</v>
-      </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I16" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="J16" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="8" t="s">
-        <v>210</v>
+      <c r="A17" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="B17" s="3">
         <v>0.59375</v>
@@ -2100,44 +3160,44 @@
         <v>0.625</v>
       </c>
       <c r="D17" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E17" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I17" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H18" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H19" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H20" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H21" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H22" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2154,10 +3214,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2171,7 +3231,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -2183,10 +3243,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -2200,6 +3260,15 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -2211,8 +3280,17 @@
       <c r="C3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.45">
+      <c r="D3" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2223,247 +3301,1471 @@
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>257</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>258</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
+      <c r="D6" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
+      <c r="D7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>214</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" t="s">
+        <v>216</v>
+      </c>
+      <c r="F8" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E10" t="s">
+        <v>219</v>
+      </c>
+      <c r="F10" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F11" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" t="s">
+        <v>226</v>
+      </c>
+      <c r="F13" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
+      <c r="D14" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E14" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E15" t="s">
+        <v>230</v>
+      </c>
+      <c r="F15" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E16" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E17" t="s">
+        <v>243</v>
+      </c>
+      <c r="F17" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" t="s">
+        <v>246</v>
+      </c>
+      <c r="F18" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>262</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>264</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E19" t="s">
+        <v>266</v>
+      </c>
+      <c r="F19" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E20" t="s">
+        <v>249</v>
+      </c>
+      <c r="F20" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E21" t="s">
+        <v>252</v>
+      </c>
+      <c r="F21" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F22" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>271</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="E23" t="s">
+        <v>256</v>
+      </c>
+      <c r="F23" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>268</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>269</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>82</v>
+        <v>270</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="E24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>85</v>
+        <v>273</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>274</v>
+      </c>
+      <c r="B25" t="s">
+        <v>275</v>
+      </c>
+      <c r="C25" t="s">
+        <v>276</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E25" t="s">
+        <v>278</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>280</v>
+      </c>
+      <c r="B26" t="s">
+        <v>281</v>
+      </c>
+      <c r="C26" t="s">
+        <v>282</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E26" t="s">
+        <v>284</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" t="s">
+        <v>287</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E27" t="s">
+        <v>289</v>
+      </c>
+      <c r="F27" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>290</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E28" t="s">
+        <v>292</v>
+      </c>
+      <c r="F28" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29" t="s">
+        <v>263</v>
+      </c>
+      <c r="C29" t="s">
+        <v>295</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E29" t="s">
+        <v>297</v>
+      </c>
+      <c r="F29" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>299</v>
+      </c>
+      <c r="B30" t="s">
+        <v>300</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E30" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>304</v>
+      </c>
+      <c r="B31" t="s">
+        <v>305</v>
+      </c>
+      <c r="C31" t="s">
+        <v>306</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E31" t="s">
+        <v>308</v>
+      </c>
+      <c r="F31" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" t="s">
+        <v>310</v>
+      </c>
+      <c r="C32" t="s">
+        <v>311</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E32" t="s">
+        <v>313</v>
+      </c>
+      <c r="F32" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>319</v>
+      </c>
+      <c r="B33" t="s">
+        <v>314</v>
+      </c>
+      <c r="C33" t="s">
+        <v>315</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E33" t="s">
+        <v>317</v>
+      </c>
+      <c r="F33" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>320</v>
+      </c>
+      <c r="B34" t="s">
+        <v>321</v>
+      </c>
+      <c r="C34" t="s">
+        <v>322</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E34" t="s">
+        <v>324</v>
+      </c>
+      <c r="F34" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>326</v>
+      </c>
+      <c r="B35" t="s">
+        <v>327</v>
+      </c>
+      <c r="C35" t="s">
+        <v>328</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E35" t="s">
+        <v>330</v>
+      </c>
+      <c r="F35" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>331</v>
+      </c>
+      <c r="B36" t="s">
+        <v>332</v>
+      </c>
+      <c r="C36" t="s">
+        <v>333</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="E36" t="s">
+        <v>335</v>
+      </c>
+      <c r="F36" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>337</v>
+      </c>
+      <c r="B37" t="s">
+        <v>338</v>
+      </c>
+      <c r="C37" t="s">
+        <v>339</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="E37" t="s">
+        <v>341</v>
+      </c>
+      <c r="F37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>342</v>
+      </c>
+      <c r="B38" t="s">
+        <v>343</v>
+      </c>
+      <c r="C38" t="s">
+        <v>344</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="F38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>347</v>
+      </c>
+      <c r="B39" t="s">
+        <v>349</v>
+      </c>
+      <c r="C39" t="s">
+        <v>350</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="F39" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>352</v>
+      </c>
+      <c r="B40" t="s">
+        <v>353</v>
+      </c>
+      <c r="C40" t="s">
+        <v>354</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="F40" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>357</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>358</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E41" t="s">
+        <v>360</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B42" t="s">
+        <v>362</v>
+      </c>
+      <c r="C42" t="s">
+        <v>363</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>366</v>
+      </c>
+      <c r="B43" t="s">
+        <v>367</v>
+      </c>
+      <c r="C43" t="s">
+        <v>368</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="E43" t="s">
+        <v>370</v>
+      </c>
+      <c r="F43" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>372</v>
+      </c>
+      <c r="B44" t="s">
+        <v>373</v>
+      </c>
+      <c r="C44" t="s">
+        <v>374</v>
+      </c>
+      <c r="D44" t="s">
+        <v>375</v>
+      </c>
+      <c r="E44" t="s">
+        <v>376</v>
+      </c>
+      <c r="F44" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>378</v>
+      </c>
+      <c r="B45" t="s">
+        <v>379</v>
+      </c>
+      <c r="C45" t="s">
+        <v>380</v>
+      </c>
+      <c r="D45" t="s">
+        <v>381</v>
+      </c>
+      <c r="E45" t="s">
+        <v>382</v>
+      </c>
+      <c r="F45" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>384</v>
+      </c>
+      <c r="B46" t="s">
+        <v>385</v>
+      </c>
+      <c r="C46" t="s">
+        <v>386</v>
+      </c>
+      <c r="E46" t="s">
+        <v>388</v>
+      </c>
+      <c r="F46" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>389</v>
+      </c>
+      <c r="B47" t="s">
+        <v>379</v>
+      </c>
+      <c r="C47" t="s">
+        <v>390</v>
+      </c>
+      <c r="D47" t="s">
+        <v>391</v>
+      </c>
+      <c r="E47" t="s">
+        <v>392</v>
+      </c>
+      <c r="F47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" t="s">
+        <v>394</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E48" t="s">
+        <v>395</v>
+      </c>
+      <c r="F48" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>397</v>
+      </c>
+      <c r="B49" t="s">
+        <v>398</v>
+      </c>
+      <c r="C49" t="s">
+        <v>399</v>
+      </c>
+      <c r="D49" t="s">
+        <v>400</v>
+      </c>
+      <c r="E49" t="s">
+        <v>401</v>
+      </c>
+      <c r="F49" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>402</v>
+      </c>
+      <c r="B50" t="s">
+        <v>403</v>
+      </c>
+      <c r="C50" t="s">
+        <v>404</v>
+      </c>
+      <c r="D50" t="s">
+        <v>405</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="F50" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>409</v>
+      </c>
+      <c r="B51" t="s">
+        <v>410</v>
+      </c>
+      <c r="C51" t="s">
+        <v>411</v>
+      </c>
+      <c r="D51" t="s">
+        <v>413</v>
+      </c>
+      <c r="E51" t="s">
+        <v>412</v>
+      </c>
+      <c r="F51" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>415</v>
+      </c>
+      <c r="B52" t="s">
+        <v>416</v>
+      </c>
+      <c r="C52" t="s">
+        <v>417</v>
+      </c>
+      <c r="D52" t="s">
+        <v>418</v>
+      </c>
+      <c r="E52" t="s">
+        <v>419</v>
+      </c>
+      <c r="F52" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>421</v>
+      </c>
+      <c r="B53" t="s">
+        <v>422</v>
+      </c>
+      <c r="C53" t="s">
+        <v>423</v>
+      </c>
+      <c r="D53" t="s">
+        <v>424</v>
+      </c>
+      <c r="E53" t="s">
+        <v>425</v>
+      </c>
+      <c r="F53" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>426</v>
+      </c>
+      <c r="B54" t="s">
+        <v>379</v>
+      </c>
+      <c r="C54" t="s">
+        <v>427</v>
+      </c>
+      <c r="D54" t="s">
+        <v>428</v>
+      </c>
+      <c r="E54" t="s">
+        <v>429</v>
+      </c>
+      <c r="F54" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>430</v>
+      </c>
+      <c r="B55" t="s">
+        <v>431</v>
+      </c>
+      <c r="C55" t="s">
+        <v>432</v>
+      </c>
+      <c r="D55" t="s">
+        <v>433</v>
+      </c>
+      <c r="E55" t="s">
+        <v>434</v>
+      </c>
+      <c r="F55" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>435</v>
+      </c>
+      <c r="B56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" t="s">
+        <v>436</v>
+      </c>
+      <c r="F56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>437</v>
+      </c>
+      <c r="B57" t="s">
+        <v>438</v>
+      </c>
+      <c r="C57" t="s">
+        <v>439</v>
+      </c>
+      <c r="D57" t="s">
+        <v>440</v>
+      </c>
+      <c r="E57" t="s">
+        <v>441</v>
+      </c>
+      <c r="F57" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>443</v>
+      </c>
+      <c r="B58" t="s">
+        <v>444</v>
+      </c>
+      <c r="C58" t="s">
+        <v>344</v>
+      </c>
+      <c r="D58" t="s">
+        <v>445</v>
+      </c>
+      <c r="E58" t="s">
+        <v>446</v>
+      </c>
+      <c r="F58" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>448</v>
+      </c>
+      <c r="B59" t="s">
+        <v>379</v>
+      </c>
+      <c r="C59" t="s">
+        <v>449</v>
+      </c>
+      <c r="D59" t="s">
+        <v>450</v>
+      </c>
+      <c r="E59" t="s">
+        <v>451</v>
+      </c>
+      <c r="F59" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>453</v>
+      </c>
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" t="s">
+        <v>454</v>
+      </c>
+      <c r="D60" t="s">
+        <v>455</v>
+      </c>
+      <c r="E60" t="s">
+        <v>456</v>
+      </c>
+      <c r="F60" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61" t="s">
+        <v>459</v>
+      </c>
+      <c r="C61" t="s">
+        <v>460</v>
+      </c>
+      <c r="D61" t="s">
+        <v>461</v>
+      </c>
+      <c r="E61" t="s">
+        <v>458</v>
+      </c>
+      <c r="F61" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>463</v>
+      </c>
+      <c r="B62" t="s">
+        <v>464</v>
+      </c>
+      <c r="C62" t="s">
+        <v>466</v>
+      </c>
+      <c r="D62" t="s">
+        <v>465</v>
+      </c>
+      <c r="E62" t="s">
+        <v>467</v>
+      </c>
+      <c r="F62" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>468</v>
+      </c>
+      <c r="B63" t="s">
+        <v>469</v>
+      </c>
+      <c r="C63" t="s">
+        <v>470</v>
+      </c>
+      <c r="D63" t="s">
+        <v>471</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="F63" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>473</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" t="s">
+        <v>474</v>
+      </c>
+      <c r="D64" t="s">
+        <v>475</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="F64" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>478</v>
+      </c>
+      <c r="B65" t="s">
+        <v>479</v>
+      </c>
+      <c r="C65" t="s">
+        <v>315</v>
+      </c>
+      <c r="D65" t="s">
+        <v>480</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="F65" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" t="s">
+        <v>338</v>
+      </c>
+      <c r="C66" t="s">
+        <v>483</v>
+      </c>
+      <c r="D66" t="s">
+        <v>484</v>
+      </c>
+      <c r="E66" t="s">
+        <v>485</v>
+      </c>
+      <c r="F66" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>487</v>
+      </c>
+      <c r="B67" t="s">
+        <v>488</v>
+      </c>
+      <c r="C67" t="s">
+        <v>489</v>
+      </c>
+      <c r="D67" t="s">
+        <v>490</v>
+      </c>
+      <c r="E67" t="s">
+        <v>491</v>
+      </c>
+      <c r="F67" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>493</v>
+      </c>
+      <c r="B68" t="s">
+        <v>494</v>
+      </c>
+      <c r="C68" t="s">
+        <v>495</v>
+      </c>
+      <c r="D68" t="s">
+        <v>496</v>
+      </c>
+      <c r="E68" t="s">
+        <v>497</v>
+      </c>
+      <c r="F68" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>498</v>
+      </c>
+      <c r="B69" t="s">
+        <v>349</v>
+      </c>
+      <c r="C69" t="s">
+        <v>500</v>
+      </c>
+      <c r="D69" t="s">
+        <v>499</v>
+      </c>
+      <c r="E69" t="s">
+        <v>501</v>
+      </c>
+      <c r="F69" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>502</v>
+      </c>
+      <c r="B70" t="s">
+        <v>503</v>
+      </c>
+      <c r="C70" t="s">
+        <v>504</v>
+      </c>
+      <c r="D70" t="s">
+        <v>505</v>
+      </c>
+      <c r="E70" t="s">
+        <v>506</v>
+      </c>
+      <c r="F70" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>507</v>
+      </c>
+      <c r="B71" t="s">
+        <v>508</v>
+      </c>
+      <c r="C71" t="s">
+        <v>276</v>
+      </c>
+      <c r="D71" t="s">
+        <v>509</v>
+      </c>
+      <c r="E71" t="s">
+        <v>510</v>
+      </c>
+      <c r="F71" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>512</v>
+      </c>
+      <c r="B72" t="s">
+        <v>379</v>
+      </c>
+      <c r="C72" t="s">
+        <v>513</v>
+      </c>
+      <c r="D72" t="s">
+        <v>514</v>
+      </c>
+      <c r="E72" t="s">
+        <v>515</v>
+      </c>
+      <c r="F72" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>516</v>
+      </c>
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" t="s">
+        <v>517</v>
+      </c>
+      <c r="D73" t="s">
+        <v>518</v>
+      </c>
+      <c r="E73" t="s">
+        <v>519</v>
+      </c>
+      <c r="F73" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>520</v>
+      </c>
+      <c r="B74" t="s">
+        <v>521</v>
+      </c>
+      <c r="C74" t="s">
+        <v>522</v>
+      </c>
+      <c r="D74" t="s">
+        <v>523</v>
+      </c>
+      <c r="E74" t="s">
+        <v>524</v>
+      </c>
+      <c r="F74" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>526</v>
+      </c>
+      <c r="B75" t="s">
+        <v>527</v>
+      </c>
+      <c r="C75" t="s">
+        <v>528</v>
+      </c>
+      <c r="D75" t="s">
+        <v>529</v>
+      </c>
+      <c r="E75" t="s">
+        <v>530</v>
+      </c>
+      <c r="F75" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="http://aiworldexpo.com/sessions/panel-putting-face-ai/"/>
+    <hyperlink ref="F3" r:id="rId2" display="http://aiworldexpo.com/sessions/ai-in-industry/"/>
+    <hyperlink ref="F9" r:id="rId3" display="http://aiworldexpo.com/sessions/evolutionordisruption/"/>
+    <hyperlink ref="F10" r:id="rId4" display="http://aiworldexpo.com/sessions/workshop-machine-learning/"/>
+    <hyperlink ref="F11" r:id="rId5" display="http://aiworldexpo.com/sessions/workshop-machine-learning/"/>
+    <hyperlink ref="F13" r:id="rId6" display="http://aiworldexpo.com/sessions/ai-executive-summit/"/>
+    <hyperlink ref="F14" r:id="rId7" display="http://aiworldexpo.com/sessions/stat-of-artificial-intelligence/"/>
+    <hyperlink ref="F15" r:id="rId8" display="http://aiworldexpo.com/sessions/keynote-2/"/>
+    <hyperlink ref="F18" r:id="rId9" display="http://aiworldexpo.com/sessions/evolutionordisruption/"/>
+    <hyperlink ref="F20" r:id="rId10" display="http://aiworldexpo.com/sessions/building-ecosystem/"/>
+    <hyperlink ref="F22" r:id="rId11" display="http://aiworldexpo.com/sessions/building-ecosystem/"/>
+    <hyperlink ref="D27" r:id="rId12" display="http://twitter.com/mikeolson"/>
+    <hyperlink ref="F27" r:id="rId13" display="http://aiworldexpo.com/sessions/keynote-3/"/>
+    <hyperlink ref="F28" r:id="rId14" display="http://aiworldexpo.com/sessions/keynote-6/"/>
+    <hyperlink ref="F29" r:id="rId15" display="http://aiworldexpo.com/sessions/keynote-luminoso/"/>
+    <hyperlink ref="E37" r:id="rId16"/>
+    <hyperlink ref="E38" r:id="rId17"/>
+    <hyperlink ref="F38" r:id="rId18" display="http://aiworldexpo.com/sessions/stat-of-artificial-intelligence/"/>
+    <hyperlink ref="E39" r:id="rId19"/>
+    <hyperlink ref="E40" r:id="rId20"/>
+    <hyperlink ref="F40" r:id="rId21" display="http://aiworldexpo.com/sessions/keynote-5/"/>
+    <hyperlink ref="F41" r:id="rId22" display="http://aiworldexpo.com/sessions/stat-of-artificial-intelligence/"/>
+    <hyperlink ref="E42" r:id="rId23"/>
+    <hyperlink ref="F42" r:id="rId24" display="http://aiworldexpo.com/sessions/2828/"/>
+    <hyperlink ref="F43" r:id="rId25" display="http://aiworldexpo.com/sessions/keynote-5/"/>
+    <hyperlink ref="F46" r:id="rId26" display="http://aiworldexpo.com/sessions/ai-technology-solutions-theater-open-attendees/"/>
+    <hyperlink ref="E50" r:id="rId27"/>
+    <hyperlink ref="F51" r:id="rId28" display="http://aiworldexpo.com/sessions/panel-real-time-intelligence-security-enterprise/"/>
+    <hyperlink ref="F52" r:id="rId29" display="http://aiworldexpo.com/sessions/ai-iot/"/>
+    <hyperlink ref="F53" r:id="rId30" display="http://aiworldexpo.com/sessions/ai-cognitive-computing-healthcare/"/>
+    <hyperlink ref="F54" r:id="rId31" display="http://aiworldexpo.com/sessions/ai-technology-solutions-theater-open-attendees/"/>
+    <hyperlink ref="E55" r:id="rId32"/>
+    <hyperlink ref="F55" r:id="rId33" display="http://aiworldexpo.com/sessions/ai-in-industry/"/>
+    <hyperlink ref="F56" r:id="rId34" display="http://aiworldexpo.com/sessions/state-of-machine-learning-3-0-ai/"/>
+    <hyperlink ref="F57" r:id="rId35" display="http://aiworldexpo.com/sessions/artificial-intelligence-meets-virtual-reality/"/>
+    <hyperlink ref="F61" r:id="rId36" display="http://aiworldexpo.com/sessions/continental-breakfast-hosted-workfusion/"/>
+    <hyperlink ref="F62" r:id="rId37" display="http://aiworldexpo.com/sessions/hpc-for-ai-ecosystem/"/>
+    <hyperlink ref="E63" r:id="rId38"/>
+    <hyperlink ref="E64" r:id="rId39"/>
+    <hyperlink ref="E65" r:id="rId40"/>
+    <hyperlink ref="F66" r:id="rId41" display="http://aiworldexpo.com/sessions/conference-wrap-up/"/>
+    <hyperlink ref="F68" r:id="rId42" display="http://aiworldexpo.com/sessions/workshop-building-bot/"/>
+    <hyperlink ref="F69" r:id="rId43" display="http://aiworldexpo.com/sessions/artificial-intelligence-meets-virtual-reality/"/>
+    <hyperlink ref="F71" r:id="rId44" display="http://aiworldexpo.com/sessions/tuesday-meetups/"/>
+    <hyperlink ref="F72" r:id="rId45" display="http://aiworldexpo.com/sessions/ai-iot/"/>
+    <hyperlink ref="E74" r:id="rId46"/>
+    <hyperlink ref="F74" r:id="rId47" display="http://aiworldexpo.com/sessions/smart-robotics-making-robots-intelligent-cognitive-aware-2/"/>
+    <hyperlink ref="F75" r:id="rId48" display="http://aiworldexpo.com/sessions/evolutionordisruption/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -2499,22 +4801,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
@@ -2524,72 +4826,72 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cross platform functionality, several fixes
</commit_message>
<xml_diff>
--- a/data/AI Conference Agenda.xlsx
+++ b/data/AI Conference Agenda.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4658" windowHeight="4380" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4658" windowHeight="4380"/>
   </bookViews>
   <sheets>
-    <sheet name="Monday AI Conference Agenda" sheetId="1" r:id="rId1"/>
+    <sheet name="AI Conference Agenda" sheetId="1" r:id="rId1"/>
     <sheet name="Tuesday AI Conference Agenda" sheetId="4" r:id="rId2"/>
     <sheet name="Speakers" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="531">
   <si>
     <t>Title</t>
   </si>
@@ -2120,10 +2120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2602,7 +2602,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>134</v>
       </c>
@@ -2664,23 +2664,513 @@
       </c>
       <c r="I18" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.34375</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D23" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D24" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E26" t="s">
+        <v>154</v>
+      </c>
+      <c r="F26" t="s">
+        <v>153</v>
+      </c>
+      <c r="G26" t="s">
+        <v>156</v>
+      </c>
+      <c r="H26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="F27" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" t="s">
+        <v>161</v>
+      </c>
+      <c r="H28" t="s">
+        <v>83</v>
+      </c>
+      <c r="I28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E29" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" t="s">
+        <v>165</v>
+      </c>
+      <c r="H29" t="s">
+        <v>83</v>
+      </c>
+      <c r="I29" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E30" t="s">
+        <v>167</v>
+      </c>
+      <c r="F30" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" t="s">
+        <v>166</v>
+      </c>
+      <c r="H30" t="s">
+        <v>83</v>
+      </c>
+      <c r="I30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" t="s">
+        <v>153</v>
+      </c>
+      <c r="G31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="D32" t="s">
+        <v>173</v>
+      </c>
+      <c r="F32" t="s">
+        <v>174</v>
+      </c>
+      <c r="H32" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C33" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E33" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" t="s">
+        <v>175</v>
+      </c>
+      <c r="H33" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" t="s">
+        <v>140</v>
+      </c>
+      <c r="J33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="D34" t="s">
+        <v>181</v>
+      </c>
+      <c r="E34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F34" t="s">
+        <v>183</v>
+      </c>
+      <c r="G34" t="s">
+        <v>184</v>
+      </c>
+      <c r="H34" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34" t="s">
+        <v>117</v>
+      </c>
+      <c r="J34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="D35" t="s">
+        <v>186</v>
+      </c>
+      <c r="E35" t="s">
+        <v>187</v>
+      </c>
+      <c r="F35" t="s">
+        <v>188</v>
+      </c>
+      <c r="G35" t="s">
+        <v>189</v>
+      </c>
+      <c r="H35" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>190</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D36" t="s">
+        <v>191</v>
+      </c>
+      <c r="E36" t="s">
+        <v>192</v>
+      </c>
+      <c r="G36" t="s">
+        <v>194</v>
+      </c>
+      <c r="H36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="C37" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D37" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" t="s">
+        <v>197</v>
+      </c>
+      <c r="F37" t="s">
+        <v>188</v>
+      </c>
+      <c r="G37" t="s">
+        <v>198</v>
+      </c>
+      <c r="H37" t="s">
+        <v>83</v>
+      </c>
+      <c r="I37" t="s">
+        <v>117</v>
+      </c>
+      <c r="J37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="C38" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D38" t="s">
+        <v>202</v>
+      </c>
+      <c r="E38" t="s">
+        <v>201</v>
+      </c>
+      <c r="F38" t="s">
+        <v>175</v>
+      </c>
+      <c r="H38" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="H43" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A18" r:id="rId1" display="http://aiworldexpo.com/sessions/enteprise-ai-adoption-open-attendees/"/>
+    <hyperlink ref="A26" r:id="rId2" display="http://aiworldexpo.com/sessions/keynote-2/"/>
+    <hyperlink ref="A33" r:id="rId3" display="http://aiworldexpo.com/sessions/finding-best-applications-ai-machine-learning/"/>
+    <hyperlink ref="A34" r:id="rId4" display="http://aiworldexpo.com/sessions/ai-future-automotive-transportation/"/>
+    <hyperlink ref="A37" r:id="rId5" display="http://aiworldexpo.com/sessions/panel-advances-machine-learning/"/>
+    <hyperlink ref="A38" r:id="rId6" display="http://aiworldexpo.com/sessions/titans-emerge-cloud-computing/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection sqref="A1:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2690,524 +3180,10 @@
     <col min="6" max="6" width="15.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>101</v>
-      </c>
+    <row r="1" spans="13:13" x14ac:dyDescent="0.45">
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.34375</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="D2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.38194444444444442</v>
-      </c>
-      <c r="D3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.38194444444444442</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.40625</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.40625</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F5" t="s">
-        <v>153</v>
-      </c>
-      <c r="G5" t="s">
-        <v>156</v>
-      </c>
-      <c r="H5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.42708333333333331</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="F6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.4548611111111111</v>
-      </c>
-      <c r="D7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F7" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.4548611111111111</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="E8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G8" t="s">
-        <v>165</v>
-      </c>
-      <c r="H8" t="s">
-        <v>83</v>
-      </c>
-      <c r="I8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.49305555555555558</v>
-      </c>
-      <c r="E9" t="s">
-        <v>167</v>
-      </c>
-      <c r="F9" t="s">
-        <v>153</v>
-      </c>
-      <c r="G9" t="s">
-        <v>166</v>
-      </c>
-      <c r="H9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.49305555555555558</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="D10" t="s">
-        <v>170</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H10" t="s">
-        <v>83</v>
-      </c>
-      <c r="I10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="D11" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" t="s">
-        <v>174</v>
-      </c>
-      <c r="H11" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" t="s">
-        <v>175</v>
-      </c>
-      <c r="H12" t="s">
-        <v>83</v>
-      </c>
-      <c r="I12" t="s">
-        <v>140</v>
-      </c>
-      <c r="J12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>180</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="D13" t="s">
-        <v>181</v>
-      </c>
-      <c r="E13" t="s">
-        <v>182</v>
-      </c>
-      <c r="F13" t="s">
-        <v>183</v>
-      </c>
-      <c r="G13" t="s">
-        <v>184</v>
-      </c>
-      <c r="H13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I13" t="s">
-        <v>117</v>
-      </c>
-      <c r="J13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>185</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="D14" t="s">
-        <v>186</v>
-      </c>
-      <c r="E14" t="s">
-        <v>187</v>
-      </c>
-      <c r="F14" t="s">
-        <v>188</v>
-      </c>
-      <c r="G14" t="s">
-        <v>189</v>
-      </c>
-      <c r="H14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B15" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="D15" t="s">
-        <v>191</v>
-      </c>
-      <c r="E15" t="s">
-        <v>192</v>
-      </c>
-      <c r="G15" t="s">
-        <v>194</v>
-      </c>
-      <c r="H15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I15" t="s">
-        <v>117</v>
-      </c>
-      <c r="J15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="D16" t="s">
-        <v>196</v>
-      </c>
-      <c r="E16" t="s">
-        <v>197</v>
-      </c>
-      <c r="F16" t="s">
-        <v>188</v>
-      </c>
-      <c r="G16" t="s">
-        <v>198</v>
-      </c>
-      <c r="H16" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" t="s">
-        <v>117</v>
-      </c>
-      <c r="J16" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="D17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E17" t="s">
-        <v>201</v>
-      </c>
-      <c r="F17" t="s">
-        <v>175</v>
-      </c>
-      <c r="H17" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="H18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="H19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="H20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="H21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="H22" t="s">
-        <v>83</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="http://aiworldexpo.com/sessions/keynote-2/"/>
-    <hyperlink ref="A12" r:id="rId2" display="http://aiworldexpo.com/sessions/finding-best-applications-ai-machine-learning/"/>
-    <hyperlink ref="A13" r:id="rId3" display="http://aiworldexpo.com/sessions/ai-future-automotive-transportation/"/>
-    <hyperlink ref="A16" r:id="rId4" display="http://aiworldexpo.com/sessions/panel-advances-machine-learning/"/>
-    <hyperlink ref="A17" r:id="rId5" display="http://aiworldexpo.com/sessions/titans-emerge-cloud-computing/"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3216,7 +3192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A60" workbookViewId="0">
       <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>

</xml_diff>